<commit_message>
test raw data to excel
</commit_message>
<xml_diff>
--- a/scripts/data-migrate/products.xlsx
+++ b/scripts/data-migrate/products.xlsx
@@ -79,1546 +79,1546 @@
     <t>brandName</t>
   </si>
   <si>
-    <t>440da91f-902b-4c9a-a37f-2f81c4ec5be0</t>
-  </si>
-  <si>
-    <t>90fb3897-d334-4e7e-b7d8-a6ffd0fa3d63</t>
-  </si>
-  <si>
-    <t>789258bb-9416-44fb-9bd3-bd4bfcb995fc</t>
-  </si>
-  <si>
-    <t>fc3a23c1-95e9-4e15-a03c-866edf43d60d</t>
-  </si>
-  <si>
-    <t>3c7a212e-90a4-4469-9662-cca5d634c6f6</t>
-  </si>
-  <si>
-    <t>35b0513e-d9c2-43b0-a0f6-254eb0ead340</t>
-  </si>
-  <si>
-    <t>185e7499-3cb6-43b9-89a1-aeb5979f0d81</t>
-  </si>
-  <si>
-    <t>7dba53fc-4f9e-479b-9064-5c1a3cdd540a</t>
-  </si>
-  <si>
-    <t>242df51a-3de2-4740-951a-861fb317719b</t>
-  </si>
-  <si>
-    <t>0f79fdc6-d2f1-453d-8e9d-bb1f96d40708</t>
-  </si>
-  <si>
-    <t>5c8b3ac0-6e42-408e-aefb-a1d1e4d151de</t>
-  </si>
-  <si>
-    <t>17f78b43-27ee-4a09-9a80-ba5493b46260</t>
-  </si>
-  <si>
-    <t>137f3b2f-a28e-4f4f-bf34-152704514750</t>
-  </si>
-  <si>
-    <t>a8b9e244-2c41-45c3-a111-f0218baabee4</t>
-  </si>
-  <si>
-    <t>ef923da3-5d2d-4586-ab24-e3999380ec33</t>
-  </si>
-  <si>
-    <t>1be1b171-f610-45ed-8a63-3faf795d5ffe</t>
-  </si>
-  <si>
-    <t>39aeed87-a627-4af6-8f04-41b08a9f4f93</t>
-  </si>
-  <si>
-    <t>df78103c-21f4-4181-ad91-7099cf637264</t>
-  </si>
-  <si>
-    <t>d96ec0c3-9c22-40ff-bfb1-15e025269500</t>
-  </si>
-  <si>
-    <t>6b48d1b9-d876-4436-b0e9-26bf2289480f</t>
-  </si>
-  <si>
-    <t>2e4a972e-2292-4526-bded-ee4dd40c5c0b</t>
-  </si>
-  <si>
-    <t>ba8c5d4f-4550-43c2-9eac-76b07e6569af</t>
-  </si>
-  <si>
-    <t>9b321d9a-f9d8-4a85-87fd-698c6a8b55cd</t>
-  </si>
-  <si>
-    <t>c7de5839-b723-4c40-b590-c5fd2596d235</t>
-  </si>
-  <si>
-    <t>ae08837f-ffbb-475d-88e3-fee1ebd325f2</t>
-  </si>
-  <si>
-    <t>87febbbf-d499-4a3a-b073-0d7d607dbac4</t>
-  </si>
-  <si>
-    <t>1bc856b0-0f17-4b59-b875-eded1283c458</t>
-  </si>
-  <si>
-    <t>e632b520-c4f6-4e19-982f-92426093cbab</t>
-  </si>
-  <si>
-    <t>d70e33ab-b368-4607-bfd6-7bf70b3954c9</t>
-  </si>
-  <si>
-    <t>c3eef36d-cf35-4747-b20c-11762d1de3e2</t>
-  </si>
-  <si>
-    <t>90f56fbe-6905-4ee2-9ec9-c6049b92ddd0</t>
-  </si>
-  <si>
-    <t>870f65bf-442f-44ca-8b5f-70ed5d2a41d8</t>
-  </si>
-  <si>
-    <t>d015f609-a7bc-4ffa-8d9f-6a44535c7642</t>
-  </si>
-  <si>
-    <t>db4deef3-5c14-49f6-9375-1020c1c6d7fb</t>
-  </si>
-  <si>
-    <t>626f11f0-9019-4350-9034-6c45b1a7bbbc</t>
-  </si>
-  <si>
-    <t>4d57c788-a366-484b-90dd-6104d8485354</t>
-  </si>
-  <si>
-    <t>e4ba2c98-0c88-4d8e-9bd3-db20f5c269aa</t>
-  </si>
-  <si>
-    <t>110d7b76-6355-4d4d-8381-085de6e15959</t>
-  </si>
-  <si>
-    <t>4870414a-0afe-4a11-ad75-47f54ca5b9b2</t>
-  </si>
-  <si>
-    <t>da2007b5-13e9-43c3-8d7c-05fd08217b6d</t>
-  </si>
-  <si>
-    <t>1ce68d91-c10b-4451-adee-e2bc3053c211</t>
-  </si>
-  <si>
-    <t>fd621ff6-a544-46a9-b8ae-4edaab577467</t>
-  </si>
-  <si>
-    <t>1fa3646c-c6c8-405f-a43b-3aff1ff1bd2d</t>
-  </si>
-  <si>
-    <t>c36cb9cc-553f-4cb0-bc7a-6f0c1c06fb45</t>
-  </si>
-  <si>
-    <t>b1ce8c45-447e-4d6e-b91b-062208beef2b</t>
-  </si>
-  <si>
-    <t>ba0a0166-6a88-4ba7-b8e3-d72da95d7891</t>
-  </si>
-  <si>
-    <t>645282d8-c72f-4be8-adec-feb35914ce64</t>
-  </si>
-  <si>
-    <t>93ef4776-8bdc-46a2-9214-3a502c21253c</t>
-  </si>
-  <si>
-    <t>f5e7f196-8239-41f0-8a3d-1d3ae0981685</t>
-  </si>
-  <si>
-    <t>6a56a619-0542-40b1-9a8e-a25988e842a1</t>
-  </si>
-  <si>
-    <t>18e6dba0-ee04-4c03-ba44-a2ade75c5f1e</t>
-  </si>
-  <si>
-    <t>97ba90a3-c08e-4d89-86fd-fe0db25dfbf6</t>
-  </si>
-  <si>
-    <t>8354045e-9ef5-4e01-aa94-62c4c787407d</t>
-  </si>
-  <si>
-    <t>df375bf5-0847-4e69-88fa-246da3e99df6</t>
-  </si>
-  <si>
-    <t>ae6815bd-2134-4236-b4e8-20bb683f61c6</t>
-  </si>
-  <si>
-    <t>69844f16-b0cd-4492-a910-1d01f96cf045</t>
-  </si>
-  <si>
-    <t>2870d7c9-faa6-411a-a0a6-008d415c025f</t>
-  </si>
-  <si>
-    <t>18666133-c141-47ba-ae29-6db5718d0aef</t>
-  </si>
-  <si>
-    <t>8ede88db-bf2a-4a8c-8cb0-6a3a00da3e10</t>
-  </si>
-  <si>
-    <t>0fdd4a20-ff09-4ca6-a29e-23aa25235530</t>
-  </si>
-  <si>
-    <t>55ec2bb3-5974-4dd7-80c8-deca8994f36e</t>
-  </si>
-  <si>
-    <t>30d5438c-793f-4876-8dd6-1e6114281b16</t>
-  </si>
-  <si>
-    <t>ac7dad86-bee2-4cd5-aa20-cbc03c7471df</t>
-  </si>
-  <si>
-    <t>7da8af6f-5b49-4634-85fc-083f1c651cbb</t>
-  </si>
-  <si>
-    <t>82229e04-494c-4938-967e-8f6bc6ab3488</t>
-  </si>
-  <si>
-    <t>03aac07e-736d-4056-8cee-0d2cd96d162e</t>
-  </si>
-  <si>
-    <t>ca4f5dbe-fbef-4a7b-8517-9db0ec78e44f</t>
-  </si>
-  <si>
-    <t>9e01fc0e-c619-4d2b-982a-914c9617bdfa</t>
-  </si>
-  <si>
-    <t>913b59bf-ae30-48e7-821b-02e199a7a407</t>
-  </si>
-  <si>
-    <t>f39ac0fd-f110-46dc-86c4-c00fa7da41bd</t>
-  </si>
-  <si>
-    <t>0c97c8ca-746e-47fa-8124-2f29d9ff28f5</t>
-  </si>
-  <si>
-    <t>c59b7871-b52c-46a9-a331-49744c943b06</t>
-  </si>
-  <si>
-    <t>76f5fb6f-ecf2-4a42-95f6-afbc593fd59b</t>
-  </si>
-  <si>
-    <t>77e729f5-3b15-4d51-b357-b1fe694917ab</t>
-  </si>
-  <si>
-    <t>8b489a85-25e9-4db8-a3b1-62e14c59a006</t>
-  </si>
-  <si>
-    <t>493e1b52-3f1c-49c7-b7c1-b9dbb79f4a62</t>
-  </si>
-  <si>
-    <t>050d7cd9-30c5-46d8-9966-0f5baa92af60</t>
-  </si>
-  <si>
-    <t>c612d478-6dfa-4731-adc5-e24bd0ed1108</t>
-  </si>
-  <si>
-    <t>ea59bd5c-59fb-43a4-9432-b50011018f8b</t>
-  </si>
-  <si>
-    <t>9ca038c1-834e-4737-910b-0dbd5d0cc0a0</t>
-  </si>
-  <si>
-    <t>657a6892-34c7-493e-9d89-44d374a863c7</t>
-  </si>
-  <si>
-    <t>1857f470-012a-4d88-a804-31252e1fc89f</t>
-  </si>
-  <si>
-    <t>7a29d6b3-d014-43f0-9e3d-16f3b289426b</t>
-  </si>
-  <si>
-    <t>3a92566e-9a9f-4e66-9f33-af8b58d740ea</t>
-  </si>
-  <si>
-    <t>73ed453f-76a9-4117-9e84-d40be32f970e</t>
-  </si>
-  <si>
-    <t>a36d9d59-c0c3-4da8-9c8d-8b5266b2bc13</t>
-  </si>
-  <si>
-    <t>e395c624-8ab1-46c2-aa6f-efc74f870b2e</t>
-  </si>
-  <si>
-    <t>7269038d-1f41-4da0-9a8c-1bf641120d1c</t>
-  </si>
-  <si>
-    <t>cb051c96-350c-4f7c-8530-882b77261bd9</t>
-  </si>
-  <si>
-    <t>a85724d3-f3d9-43cd-b443-f48a68b648bc</t>
-  </si>
-  <si>
-    <t>0d43247e-59c0-4873-8d10-8a01906ddd4f</t>
-  </si>
-  <si>
-    <t>05039ee6-1c2b-4e19-8c09-49a8740ff77b</t>
-  </si>
-  <si>
-    <t>afe783b3-26da-4f32-b051-4f6e79b470c7</t>
-  </si>
-  <si>
-    <t>1d3325a7-8e6b-4f3d-b3eb-b2484aed3308</t>
-  </si>
-  <si>
-    <t>3a254277-b93b-4357-bf41-598a1e25113d</t>
-  </si>
-  <si>
-    <t>d6c315fa-0d9f-4160-8fb3-de702a291dbe</t>
-  </si>
-  <si>
-    <t>8fca66e5-6bf6-4770-86fc-566ecd542d33</t>
-  </si>
-  <si>
-    <t>f244910c-3ac4-4454-b2d5-df5338260018</t>
-  </si>
-  <si>
-    <t>4108c682-3d53-40c1-aa98-b617803d7315</t>
-  </si>
-  <si>
-    <t>d08cea1f-3e36-4e95-b0e6-6eebe4b52d41</t>
-  </si>
-  <si>
-    <t>0c00b1bd-68fc-4d8f-9c12-5a2c869b15d5</t>
-  </si>
-  <si>
-    <t>56a3c844-3f91-4872-9646-0ece968077e9</t>
-  </si>
-  <si>
-    <t>615e83a8-5c60-4112-afb6-2154d3a7dd77</t>
-  </si>
-  <si>
-    <t>a2aa5a71-4887-464b-9fde-4c73c54e9e4a</t>
-  </si>
-  <si>
-    <t>d32cdfd6-cf64-4989-b747-23ce9228667a</t>
-  </si>
-  <si>
-    <t>a4df48df-1114-4ffa-b1f7-99ea4c2e92bd</t>
-  </si>
-  <si>
-    <t>5089af6b-1158-49de-8186-729aa6222e9c</t>
-  </si>
-  <si>
-    <t>f8b5ee28-d774-4493-8245-e64f169671e5</t>
-  </si>
-  <si>
-    <t>80f0d3d5-0bef-41fc-80af-d7ccfb59a861</t>
-  </si>
-  <si>
-    <t>9a831f4e-5265-4642-a25c-9beaeecffa3f</t>
-  </si>
-  <si>
-    <t>75406243-26ca-4367-95b0-7d5b94859636</t>
-  </si>
-  <si>
-    <t>72251710-abab-4cd9-a4e9-504d1f167b23</t>
-  </si>
-  <si>
-    <t>96df4a9d-d133-49db-be8b-e55a6ee23a35</t>
-  </si>
-  <si>
-    <t>2fb1f44c-0973-4be1-aa3b-70b57629f6bb</t>
-  </si>
-  <si>
-    <t>d49b5786-5652-49a9-82fd-17d6067d964e</t>
-  </si>
-  <si>
-    <t>9cd545fe-d2bf-4de4-b1d6-ab14f624103d</t>
-  </si>
-  <si>
-    <t>62651972-e65e-4ae9-85ef-66af8e098aa9</t>
-  </si>
-  <si>
-    <t>f18e6e1c-f012-4514-92a8-f2e345d90329</t>
-  </si>
-  <si>
-    <t>1366e0bf-6597-48c1-b0c0-832a7aa69d3f</t>
-  </si>
-  <si>
-    <t>4980455b-a4bd-4ad5-b770-de8221ab3388</t>
-  </si>
-  <si>
-    <t>ac88a9da-ab0d-4ab0-be61-5ce4b6f0191e</t>
-  </si>
-  <si>
-    <t>7a584777-ed08-4576-9fcf-dc78e488832e</t>
-  </si>
-  <si>
-    <t>13271e6b-97b6-43ec-9ebb-fdf8443b8362</t>
-  </si>
-  <si>
-    <t>c6f5b3d4-932b-4f14-b321-2695eb5b444b</t>
-  </si>
-  <si>
-    <t>a7b08840-2420-416b-bfa2-bac89863bab8</t>
-  </si>
-  <si>
-    <t>82ea4ecb-402e-4821-b42c-ebdbda8896f6</t>
-  </si>
-  <si>
-    <t>556e38e5-12c2-4443-bd2f-46096616600a</t>
-  </si>
-  <si>
-    <t>c2d970ea-2a23-4cba-bf14-b6d77ec7650c</t>
-  </si>
-  <si>
-    <t>0477cf57-6499-4a76-b3bc-63021b76441e</t>
-  </si>
-  <si>
-    <t>9115d96a-81eb-424f-9c4c-243d753d3a71</t>
-  </si>
-  <si>
-    <t>0e309689-d4ef-4237-af39-1b741473d7f4</t>
-  </si>
-  <si>
-    <t>e6ed95ba-9dd4-48b1-a4eb-5d4880ce5c2e</t>
-  </si>
-  <si>
-    <t>f36f3649-c662-417a-acda-d6797497ac00</t>
-  </si>
-  <si>
-    <t>0d371daa-38a3-4e78-9506-0f9b0b533f10</t>
-  </si>
-  <si>
-    <t>61aeadcf-f223-46b3-8c05-15cdf53b4470</t>
-  </si>
-  <si>
-    <t>f48094a1-8a6c-4222-a4cc-114b13b5ccd7</t>
-  </si>
-  <si>
-    <t>a63d64f9-adcf-4309-9f4c-6ee2ab0adfe4</t>
-  </si>
-  <si>
-    <t>f5174636-a95f-40c3-bf29-fcfcec54c3b3</t>
-  </si>
-  <si>
-    <t>b810fe10-b5c6-402a-91d0-b348d815b06b</t>
-  </si>
-  <si>
-    <t>d9114d65-f674-4c1f-880e-c76df7b1153b</t>
-  </si>
-  <si>
-    <t>386043d3-379b-4bb6-b676-d0d80d9d5a75</t>
-  </si>
-  <si>
-    <t>df27b3b0-3058-47d4-b396-8fe51af09b40</t>
-  </si>
-  <si>
-    <t>61d5878b-16ad-465a-8dc8-c2b29bdb8ef7</t>
-  </si>
-  <si>
-    <t>97ccd6a4-a467-4550-8965-cd0140c06a83</t>
-  </si>
-  <si>
-    <t>484a484c-6843-4e62-bea4-e0c99dc41c5b</t>
-  </si>
-  <si>
-    <t>0d9115b0-a73d-466e-ba4b-5ad21c5a452a</t>
-  </si>
-  <si>
-    <t>ac0ba227-2265-4435-a744-a46c8cd00e16</t>
-  </si>
-  <si>
-    <t>0dfe8f39-7040-4738-a194-f9f2e25b3f48</t>
-  </si>
-  <si>
-    <t>28423d0d-0eeb-4184-b4d0-23e05d08bab6</t>
-  </si>
-  <si>
-    <t>28569574-49e8-4ced-b015-673be37bc18a</t>
-  </si>
-  <si>
-    <t>05e8bf39-f240-434b-aa2f-643765c6b03b</t>
-  </si>
-  <si>
-    <t>0394bc19-bff4-46e7-bb9f-915fa51d42d1</t>
-  </si>
-  <si>
-    <t>6f8661b6-5030-40f3-8f72-cc3eaa8a307f</t>
-  </si>
-  <si>
-    <t>bf197c65-a6f2-4d94-b27e-77d4c02baedd</t>
-  </si>
-  <si>
-    <t>15c84e0d-b04d-4fbd-9151-f87477b6bf94</t>
-  </si>
-  <si>
-    <t>2dbb5e5d-dc34-4e05-997f-d0e853b6fbe4</t>
-  </si>
-  <si>
-    <t>1100534f-da85-4039-b304-120cff6bf9b8</t>
-  </si>
-  <si>
-    <t>34bbe8ce-7b22-4aad-893a-64d843b06616</t>
-  </si>
-  <si>
-    <t>a14e5609-5d90-427c-9803-d0d600342213</t>
-  </si>
-  <si>
-    <t>f2279463-97f0-4496-99ae-00b457735bfa</t>
-  </si>
-  <si>
-    <t>066400fd-1dc0-413d-b36a-e7f45ccc625b</t>
-  </si>
-  <si>
-    <t>bee50522-cb60-4d0c-99fd-7b2f8dc02294</t>
-  </si>
-  <si>
-    <t>20e7d925-eb0e-4976-9a28-3a2accc8b453</t>
-  </si>
-  <si>
-    <t>5448d944-0c84-4246-bd7e-5a865a9cba41</t>
-  </si>
-  <si>
-    <t>2f16c955-f2f4-4be3-8d56-1fe453804f09</t>
-  </si>
-  <si>
-    <t>51788420-1d06-47ed-9d8c-e9d0d1a0c286</t>
-  </si>
-  <si>
-    <t>6460ebd9-d939-4ebd-85c1-27b55b3398b3</t>
-  </si>
-  <si>
-    <t>46bfcce0-d88f-40e9-a436-7c4a3adc74c2</t>
-  </si>
-  <si>
-    <t>aecdc9b7-ea78-4c7f-8bb2-b5d1fd342e2e</t>
-  </si>
-  <si>
-    <t>9403aa4d-a885-401b-83c3-f98f5a9e5984</t>
-  </si>
-  <si>
-    <t>749e0b65-1a32-46c9-a0e8-ab1bc33fed5c</t>
-  </si>
-  <si>
-    <t>bd5c693d-825b-4be1-9fe9-6c494709b4a7</t>
-  </si>
-  <si>
-    <t>af7ce373-77ca-4a21-928b-1b88a7e2257e</t>
-  </si>
-  <si>
-    <t>f014fa44-464f-49c0-8693-d8ca09f1e787</t>
-  </si>
-  <si>
-    <t>3cba3e54-1fa7-40fd-ad13-bdbf74aaa4e0</t>
-  </si>
-  <si>
-    <t>f216f3ff-8254-4aa4-badd-bafa5d36ad86</t>
-  </si>
-  <si>
-    <t>bc4af89b-2724-495d-a4b1-9005727df2f6</t>
-  </si>
-  <si>
-    <t>ede974f3-f278-4bea-b7fc-c9fe5a04a08c</t>
-  </si>
-  <si>
-    <t>256fc914-460a-481b-a8c3-629ba8b83867</t>
-  </si>
-  <si>
-    <t>852d664b-ebdf-4475-9c23-4b1c4d00a028</t>
-  </si>
-  <si>
-    <t>3daa3b67-b6e4-4668-9d79-e7fcf90cf9df</t>
-  </si>
-  <si>
-    <t>7280da74-e89a-41c2-9075-68a1d7587a8b</t>
-  </si>
-  <si>
-    <t>379efd90-b495-4fe7-93aa-04f02d1ccfa0</t>
-  </si>
-  <si>
-    <t>d030a3c2-3506-4287-aab8-c882fc45f0c9</t>
-  </si>
-  <si>
-    <t>65d93ddb-f40b-42aa-956d-3b2651ddd448</t>
-  </si>
-  <si>
-    <t>a63b22d7-5abc-4e3e-90e9-57deef9b0fd0</t>
-  </si>
-  <si>
-    <t>56e9875c-b5db-4245-a31b-85314f34b5a0</t>
-  </si>
-  <si>
-    <t>be020e80-cc4c-4526-80e4-69f1a366d0e9</t>
-  </si>
-  <si>
-    <t>07c39ac1-00ee-4d6e-9eb1-eab53c2e50ad</t>
-  </si>
-  <si>
-    <t>ced2d837-ab48-48f0-8315-0cbe23076aae</t>
-  </si>
-  <si>
-    <t>f8eaf200-d1b0-4cde-b8a0-a24cca4bb8d4</t>
-  </si>
-  <si>
-    <t>f81ed0c8-bd01-4473-b8dd-8ec2e60fc057</t>
-  </si>
-  <si>
-    <t>93855d25-8e7a-4c04-98a4-b85b0f764403</t>
-  </si>
-  <si>
-    <t>c80e58f7-ca78-4e5c-9f47-f27f8672cb40</t>
-  </si>
-  <si>
-    <t>39683105-09b7-4e98-a821-a575a205eece</t>
-  </si>
-  <si>
-    <t>ff9626f6-e2d1-4da8-b4e1-e95b24acaeaf</t>
-  </si>
-  <si>
-    <t>bf6ab902-5e8c-4eea-b24f-95591e99c03a</t>
-  </si>
-  <si>
-    <t>3b3e6413-9d0a-4ce4-9993-c4cd81db5f3e</t>
-  </si>
-  <si>
-    <t>f90e25eb-d983-45ac-a742-7d0d10d0ae4d</t>
-  </si>
-  <si>
-    <t>59b129af-a3ef-42e8-8be8-9168a3b73abc</t>
-  </si>
-  <si>
-    <t>65b0c8d9-7889-408b-b5fb-db4062b4bb1d</t>
-  </si>
-  <si>
-    <t>35dcf27b-8c53-4667-98fc-729e55185e2f</t>
-  </si>
-  <si>
-    <t>ad34aeea-609b-49b7-8740-4a7615775683</t>
-  </si>
-  <si>
-    <t>c3846b16-75ea-4859-be80-f8e7c9ee457e</t>
-  </si>
-  <si>
-    <t>41fc4378-33c5-4730-8163-475a8d28cc21</t>
-  </si>
-  <si>
-    <t>2a1ac4fa-cef0-4a86-8a76-6ea1f342406d</t>
-  </si>
-  <si>
-    <t>4810241b-1a31-4c17-8a65-f7a55191d7aa</t>
-  </si>
-  <si>
-    <t>0761ab26-d64e-411a-9e41-f2792ab780b0</t>
-  </si>
-  <si>
-    <t>2647f87a-a9cd-43b1-9655-9533db7569cf</t>
-  </si>
-  <si>
-    <t>67d93da7-1603-4b4c-ae86-0cc853f9a9a7</t>
-  </si>
-  <si>
-    <t>64e9d4fa-b89d-4ae9-a222-ad4cd4a251d3</t>
-  </si>
-  <si>
-    <t>2476b864-a73f-402e-8398-b018a44efab2</t>
-  </si>
-  <si>
-    <t>f01a4122-9fe9-416d-b74e-12956aca6d45</t>
-  </si>
-  <si>
-    <t>9a13b2b4-f9f4-443f-92e6-7161883e7301</t>
-  </si>
-  <si>
-    <t>17b2f220-d61a-4259-a502-73a35ad2e91d</t>
-  </si>
-  <si>
-    <t>00ba02b3-7f66-48fc-a252-6a5898589a1d</t>
-  </si>
-  <si>
-    <t>b813a94a-aeb0-44aa-acb8-b3bfc0cb9763</t>
-  </si>
-  <si>
-    <t>cdb728df-ee0a-4156-a1cc-11fced7b64da</t>
-  </si>
-  <si>
-    <t>4e68c359-c6c0-4afa-a20f-aec712164464</t>
-  </si>
-  <si>
-    <t>1c31bbfa-3fbe-4c06-908e-c977d0ab180e</t>
-  </si>
-  <si>
-    <t>94ee0341-1bd9-46c2-aea6-f4e1909ecbe5</t>
-  </si>
-  <si>
-    <t>e1ed1e80-b239-4e9f-9b42-0a51f67dfaba</t>
-  </si>
-  <si>
-    <t>170e8f73-cf86-4fde-9d36-327e1f499405</t>
-  </si>
-  <si>
-    <t>cd5dea83-f2d7-49bc-98ce-12e6ce15107d</t>
-  </si>
-  <si>
-    <t>27bb535a-0d5f-4985-9926-7bb87d1528d1</t>
-  </si>
-  <si>
-    <t>36825688-11d9-4f0c-960e-a90fb628c793</t>
-  </si>
-  <si>
-    <t>bb688264-95cd-4b0b-a41d-d3b9a54bab88</t>
-  </si>
-  <si>
-    <t>8c9320f5-a503-4ba8-9c5a-edb3f3baf6ed</t>
-  </si>
-  <si>
-    <t>caaa9716-bcf4-4029-9955-320b952b2e3f</t>
-  </si>
-  <si>
-    <t>1ec8efe0-630c-48e3-aaa1-b76bb6958bf7</t>
-  </si>
-  <si>
-    <t>aa922638-f554-4207-9f5c-9394e1521a33</t>
-  </si>
-  <si>
-    <t>22df213e-02ed-45de-b216-e8ed88533be7</t>
-  </si>
-  <si>
-    <t>c1d32d87-2400-4e1d-9dac-04d38fdfd098</t>
-  </si>
-  <si>
-    <t>ca8b7dca-d442-4aed-99f8-25f2bcc3a20f</t>
-  </si>
-  <si>
-    <t>d5e83f54-69a0-4a5b-9886-5ffa57525b1a</t>
-  </si>
-  <si>
-    <t>24b2dd34-6251-42fc-86d5-39db844ac0cf</t>
-  </si>
-  <si>
-    <t>452e79e9-df9e-41f9-ba60-4bd8bc9fe003</t>
-  </si>
-  <si>
-    <t>2abaf4ac-710c-461a-8ba3-e2971918cd4b</t>
-  </si>
-  <si>
-    <t>a6688871-afbd-450b-97b5-5985a00bdaba</t>
-  </si>
-  <si>
-    <t>2ebd768b-c2ae-4c5c-a897-8972af1bcd23</t>
-  </si>
-  <si>
-    <t>f492f17f-0b26-40fe-985c-980021f3b10d</t>
-  </si>
-  <si>
-    <t>d472db90-ecbd-47b8-b3d6-37fe7b004f2e</t>
-  </si>
-  <si>
-    <t>7be3fe59-ee5f-4d55-9465-15006723aa0c</t>
-  </si>
-  <si>
-    <t>dd748d29-6a6b-43dc-a5ef-69ab88dd4dac</t>
-  </si>
-  <si>
-    <t>69b4bcb2-269a-43be-bc31-67e6c807d5d7</t>
-  </si>
-  <si>
-    <t>eb1f3115-5c09-4891-a744-9563529f8aea</t>
-  </si>
-  <si>
-    <t>229a8c40-dee9-461e-b478-123c7f0f463b</t>
-  </si>
-  <si>
-    <t>1c1ad877-8b19-4ff3-8bf6-e6430817435d</t>
-  </si>
-  <si>
-    <t>5b8b70df-a55a-4136-99c5-2ec2b96cc0cf</t>
-  </si>
-  <si>
-    <t>72e35bc4-92e7-4680-9a33-81e57dd2f0b8</t>
-  </si>
-  <si>
-    <t>8a4b375c-8df2-455b-bd5f-ed57a87458c6</t>
-  </si>
-  <si>
-    <t>5b297a3c-2000-4bc8-b2a8-1f32486a46f3</t>
-  </si>
-  <si>
-    <t>c0cb9304-85fe-43fb-9321-174cc39d0546</t>
-  </si>
-  <si>
-    <t>ad9786da-452e-4c2b-ae5e-4b5f86a9b04d</t>
-  </si>
-  <si>
-    <t>d2743264-c023-4a47-95ee-1ff7efa61eb8</t>
-  </si>
-  <si>
-    <t>5c80526f-7a92-454a-be68-385b1153d76d</t>
-  </si>
-  <si>
-    <t>e2bc2ee6-6272-43a4-83ad-bf16558721b5</t>
-  </si>
-  <si>
-    <t>db30c5f0-2990-40b5-b9f1-7061266ba830</t>
-  </si>
-  <si>
-    <t>225f05e9-79db-431d-93bf-254e53f38e9c</t>
-  </si>
-  <si>
-    <t>e712a151-b773-47a4-a76b-f3ae4e1910fa</t>
-  </si>
-  <si>
-    <t>bd14ac41-bde6-4dfe-b7d3-34f04d159e32</t>
-  </si>
-  <si>
-    <t>2d77dc0b-a62a-4143-9e4b-cdbbfbd346f5</t>
-  </si>
-  <si>
-    <t>4f877299-22c4-4d7a-bf6e-7a8cf3f1bd76</t>
-  </si>
-  <si>
-    <t>92646d6f-d4a1-47cd-a431-fa3abfa6242d</t>
-  </si>
-  <si>
-    <t>eddb11c8-aca4-41b1-8820-e80cb46caf6f</t>
-  </si>
-  <si>
-    <t>cc95fbbd-0acc-48e3-80bc-0d66d01ee69a</t>
-  </si>
-  <si>
-    <t>2925cdc2-c4f3-415b-8aa5-5cfa00ef5559</t>
-  </si>
-  <si>
-    <t>16c48ebf-31ac-4a4c-a06f-026e581759d1</t>
-  </si>
-  <si>
-    <t>4485197c-345a-47cc-9ed0-d963f90cbb55</t>
-  </si>
-  <si>
-    <t>802f298e-bec5-4963-b581-f8564ffd56a1</t>
-  </si>
-  <si>
-    <t>a7321523-1d93-4de2-851f-e145a60c15cb</t>
-  </si>
-  <si>
-    <t>3873687f-b0e7-41eb-9c74-a19d0d4cf00b</t>
-  </si>
-  <si>
-    <t>d70105c7-f33f-4e67-9371-f3cf92e3e430</t>
-  </si>
-  <si>
-    <t>4259db90-3e42-45b4-ba77-8434545950f5</t>
-  </si>
-  <si>
-    <t>7b526ba7-2271-4a8e-922a-9e5416c09e1b</t>
-  </si>
-  <si>
-    <t>b13e6a5f-f69b-451b-bd59-d77fde32a1f0</t>
-  </si>
-  <si>
-    <t>2b03c114-58ea-4f95-bc23-7505cd9fa263</t>
-  </si>
-  <si>
-    <t>22fc3d82-c412-4cda-b854-4ae220280c20</t>
-  </si>
-  <si>
-    <t>ed31aa8d-d395-43b8-953e-6ff89daa149d</t>
-  </si>
-  <si>
-    <t>7fde26e1-529c-4430-adc5-b450df4c9f17</t>
-  </si>
-  <si>
-    <t>13fba698-e5b0-47ba-a697-44fa32654e93</t>
-  </si>
-  <si>
-    <t>444b9125-010a-4168-a8d3-a2c68593cd42</t>
-  </si>
-  <si>
-    <t>00dda9cc-b74d-4be3-9af2-8026f41e28f4</t>
-  </si>
-  <si>
-    <t>d261d886-6fd2-4a53-9714-1904303d27d2</t>
-  </si>
-  <si>
-    <t>7fd2ef38-f456-4c4c-bba0-93d1457df7d4</t>
-  </si>
-  <si>
-    <t>cbdfe715-c10d-44f2-a5e1-71be7bf252ed</t>
-  </si>
-  <si>
-    <t>7d21e826-3b6a-424f-801f-018a5c84ef5e</t>
-  </si>
-  <si>
-    <t>df63e38c-2559-40ad-9ee5-c01b55a3a9f0</t>
-  </si>
-  <si>
-    <t>ceab18d7-a0f3-4fef-b6e8-df239391f350</t>
-  </si>
-  <si>
-    <t>ebcb42da-b6a5-440a-8e24-5ae4cb2b6eb6</t>
-  </si>
-  <si>
-    <t>9b3088ae-7591-4158-943b-2146a2be5827</t>
-  </si>
-  <si>
-    <t>ed0a1d63-8889-42f8-bc9a-6e54bf275bc9</t>
-  </si>
-  <si>
-    <t>84ce9b05-64c5-4890-bc24-4ae6217c99b7</t>
-  </si>
-  <si>
-    <t>ff38f193-4df2-4c32-b218-88285510cb45</t>
-  </si>
-  <si>
-    <t>42bfc590-a81a-4b33-9fd7-594fd86d02cc</t>
-  </si>
-  <si>
-    <t>d65f895f-e687-43f5-a5af-aae1734cf075</t>
-  </si>
-  <si>
-    <t>c62f0923-46ff-495e-b3fe-2b5efb638b10</t>
-  </si>
-  <si>
-    <t>3e93871f-324e-4e9d-8187-8d5b7b95251e</t>
-  </si>
-  <si>
-    <t>09359dfd-fd24-44a9-b765-ad37ec8e5ccf</t>
-  </si>
-  <si>
-    <t>109b11f5-7eb2-48e3-b122-9bf03c0b9faf</t>
-  </si>
-  <si>
-    <t>e2135614-6964-496b-aadb-9a5cfdc19aad</t>
-  </si>
-  <si>
-    <t>0e75e1e4-a6b7-4e7f-b603-b79a21e864cd</t>
-  </si>
-  <si>
-    <t>26dc9bee-4fe4-4085-b5b7-c4beb69d4e9d</t>
-  </si>
-  <si>
-    <t>59a331e3-c02c-4992-9b92-ce002fd27848</t>
-  </si>
-  <si>
-    <t>2594d278-fcec-4a70-a78d-8abaf72c92a6</t>
-  </si>
-  <si>
-    <t>190a8b13-e851-4004-8f3f-3b76f6015766</t>
-  </si>
-  <si>
-    <t>3ca290b1-5ad0-419c-a4a9-cc34ef5f83e6</t>
-  </si>
-  <si>
-    <t>9e74b124-726a-4cb2-b984-776dd4f02162</t>
-  </si>
-  <si>
-    <t>0298ccab-f8e3-499f-a60f-7fc8cd48310a</t>
-  </si>
-  <si>
-    <t>b3f68e07-d804-46c8-9e80-dba252d3dbc5</t>
-  </si>
-  <si>
-    <t>a43cde0b-1702-4c29-b4f6-854e3be6f0e3</t>
-  </si>
-  <si>
-    <t>bc0b62f0-082e-4006-9405-795280d9f13e</t>
-  </si>
-  <si>
-    <t>8de24694-f6d1-4adf-9d71-5b2fc0783836</t>
-  </si>
-  <si>
-    <t>47f0d8ba-6011-47d6-8fac-970af799f7a0</t>
-  </si>
-  <si>
-    <t>124b7ab5-8c5e-47ed-a492-7531b181f555</t>
-  </si>
-  <si>
-    <t>110c87f2-ebc5-48a1-8f9f-7502de371811</t>
-  </si>
-  <si>
-    <t>ce8ee2c8-7ae2-495c-8e3b-31479bc54da3</t>
-  </si>
-  <si>
-    <t>a8f61ebb-7599-4969-b1e2-f74a57f467f2</t>
-  </si>
-  <si>
-    <t>cfdf2320-634d-4987-ae4c-4f1b55be4f4d</t>
-  </si>
-  <si>
-    <t>a7205a8b-2412-45dd-abb8-4f452378d8a5</t>
-  </si>
-  <si>
-    <t>2b0d6aed-899d-46b8-b75b-5031d55c98b5</t>
-  </si>
-  <si>
-    <t>6976ab3c-ae80-4e24-9489-5c85e1a649e7</t>
-  </si>
-  <si>
-    <t>6eed66a1-0887-4b7c-b019-8846c257bb4e</t>
-  </si>
-  <si>
-    <t>ca25fb84-f3d2-4791-8bd3-00008e0c020c</t>
-  </si>
-  <si>
-    <t>2571653f-3a51-43e2-9574-9788c8806d2e</t>
-  </si>
-  <si>
-    <t>6f95e191-c06c-4566-af52-0eac40bdcac2</t>
-  </si>
-  <si>
-    <t>db1f74a9-49d8-4128-9558-938d475e9ba9</t>
-  </si>
-  <si>
-    <t>1203b581-4a62-47ce-89b5-9c639d711641</t>
-  </si>
-  <si>
-    <t>c1fed596-0244-4406-86bd-cf84bb5bb2e5</t>
-  </si>
-  <si>
-    <t>19b8b0d0-ce7d-4088-9619-2c6b067a0d52</t>
-  </si>
-  <si>
-    <t>4a4763c6-3921-4de5-a4ea-868232f692b5</t>
-  </si>
-  <si>
-    <t>40e862d5-577c-47ce-8c44-7eb82a394aae</t>
-  </si>
-  <si>
-    <t>7edc0917-3126-4aea-b287-40f3fdcc5dd3</t>
-  </si>
-  <si>
-    <t>0a9686a9-ed1b-4ee6-b276-f37812470d31</t>
-  </si>
-  <si>
-    <t>047e1906-7465-4a88-a7c9-28b5b03cf657</t>
-  </si>
-  <si>
-    <t>fc630f4c-1b5b-4725-b498-463e68293903</t>
-  </si>
-  <si>
-    <t>dc782382-b3d4-4df9-8c1c-b72d79537662</t>
-  </si>
-  <si>
-    <t>7eb479cb-9d81-48df-84a6-26be76518ec8</t>
-  </si>
-  <si>
-    <t>c7b0e592-f95c-4cb3-8ea3-81e6a4a761e9</t>
-  </si>
-  <si>
-    <t>a1938333-a655-4664-97a1-4a993aeae070</t>
-  </si>
-  <si>
-    <t>da76d8d5-f7e6-4f53-aa42-76fa46a33bac</t>
-  </si>
-  <si>
-    <t>44ff2df5-693e-409a-9d4c-4fc1e9b2f24a</t>
-  </si>
-  <si>
-    <t>1c501c45-be02-4103-bf45-e441f853c45b</t>
-  </si>
-  <si>
-    <t>cdd7ab2b-390a-4490-b42e-f4d1c952a951</t>
-  </si>
-  <si>
-    <t>f9b306dd-8239-469b-90cd-210e7e04e400</t>
-  </si>
-  <si>
-    <t>b82a5ffd-1f1e-4de4-9299-05ebf8b5c617</t>
-  </si>
-  <si>
-    <t>77033baf-2068-4f78-bc24-e35a4ce61fa3</t>
-  </si>
-  <si>
-    <t>f8f5b38b-454b-4e3e-a1a3-441ba44afcf3</t>
-  </si>
-  <si>
-    <t>9d077c79-9870-4abf-a476-9a3dfd895f22</t>
-  </si>
-  <si>
-    <t>96a7d83c-b06e-4042-aaf5-3c7e01f9e4f9</t>
-  </si>
-  <si>
-    <t>7fce97b2-d406-4576-991b-bb6de226b8d0</t>
-  </si>
-  <si>
-    <t>104281e3-73b8-43e1-8e46-9bbf4f98fb24</t>
-  </si>
-  <si>
-    <t>17141a77-9aa9-4ab8-b434-e8dc18ba248f</t>
-  </si>
-  <si>
-    <t>30830fd8-ff45-4ab9-b117-45e60678d92f</t>
-  </si>
-  <si>
-    <t>e84dec5b-f297-4832-9e33-ece7baafedcd</t>
-  </si>
-  <si>
-    <t>ea459dde-5306-4b18-b649-bd1ec3f660da</t>
-  </si>
-  <si>
-    <t>a73bd487-b4a0-4db6-8b68-9a5144e6ee0b</t>
-  </si>
-  <si>
-    <t>400f1034-46d1-4d89-816a-b8df1ca816a6</t>
-  </si>
-  <si>
-    <t>bb8e2862-0edf-4386-8870-eff80aae873a</t>
-  </si>
-  <si>
-    <t>9fb5af93-7c34-4609-8fa8-cf90a6ab9d00</t>
-  </si>
-  <si>
-    <t>2f47270d-149b-4256-a812-ab369b2d09ee</t>
-  </si>
-  <si>
-    <t>9e2a0f84-27f7-4fc4-988f-0393ca1415a3</t>
-  </si>
-  <si>
-    <t>6d35d21c-b8b8-48a2-9d13-1b7c73a0e74a</t>
-  </si>
-  <si>
-    <t>cbd4976d-bca3-4225-862a-f6c3e18c3579</t>
-  </si>
-  <si>
-    <t>60aaef46-970a-4402-aadc-06c4b732570a</t>
-  </si>
-  <si>
-    <t>c7dec6af-ac15-4aa8-a002-bb2bef802e65</t>
-  </si>
-  <si>
-    <t>6cdad34b-e158-43c4-9f1e-0f50c8fb0e72</t>
-  </si>
-  <si>
-    <t>fa92904c-026e-45ef-942b-84de1caf1252</t>
-  </si>
-  <si>
-    <t>caedf881-2e52-409a-af8b-ab53c806700c</t>
-  </si>
-  <si>
-    <t>c9feae6b-1bcb-4045-b117-056c095011e4</t>
-  </si>
-  <si>
-    <t>32416645-e12f-47c7-b513-f50ffd642f9c</t>
-  </si>
-  <si>
-    <t>178e5e63-8b95-4156-9279-fd0408c64224</t>
-  </si>
-  <si>
-    <t>08f8b494-072f-47db-9b88-51dffff579d9</t>
-  </si>
-  <si>
-    <t>37802718-2a75-488f-b862-1080adbd4b54</t>
-  </si>
-  <si>
-    <t>a9334fbd-d59a-4032-b8b2-ed14f004f223</t>
-  </si>
-  <si>
-    <t>9ad609fe-de8d-49c2-ad25-dbabe724ffaf</t>
-  </si>
-  <si>
-    <t>21e3588d-f6e7-4d45-9ce4-8f5ba8fdcfd2</t>
-  </si>
-  <si>
-    <t>f3b16c44-fe11-4778-8d57-a16d44a71e2a</t>
-  </si>
-  <si>
-    <t>877d305f-500a-4dcd-a324-b0e7d1cb129e</t>
-  </si>
-  <si>
-    <t>6ffb7e16-5492-4257-81df-ef8667723237</t>
-  </si>
-  <si>
-    <t>8964a156-149c-460a-8268-b3e58fbae590</t>
-  </si>
-  <si>
-    <t>9951b446-6a17-4351-a10c-57c85979796a</t>
-  </si>
-  <si>
-    <t>323111f3-0410-4564-9a19-cd66321e9dc3</t>
-  </si>
-  <si>
-    <t>f36bb176-4f0b-411f-99a7-2b9b7df4091e</t>
-  </si>
-  <si>
-    <t>31400250-6926-4d33-a0f0-4b356127f0aa</t>
-  </si>
-  <si>
-    <t>a3a4d024-5814-41f0-9ede-17402f75c16e</t>
-  </si>
-  <si>
-    <t>bffff469-8d6a-4880-b78a-aabd79434ad4</t>
-  </si>
-  <si>
-    <t>20a2c753-11d9-4338-bed8-abf56a50d8ea</t>
-  </si>
-  <si>
-    <t>630a59de-5ffe-46ec-addc-777778d1d5bc</t>
-  </si>
-  <si>
-    <t>ad0900b3-b083-45d7-812f-232a4104a21e</t>
-  </si>
-  <si>
-    <t>18a6c7ab-cf1d-45a9-a461-38951f104e70</t>
-  </si>
-  <si>
-    <t>035478cc-b987-4fc0-a850-556ce929ce78</t>
-  </si>
-  <si>
-    <t>be0608ce-bfce-4655-ad26-0591d1c0edb7</t>
-  </si>
-  <si>
-    <t>0a63a1ea-cbf5-41b6-87e1-4e70369fe2ce</t>
-  </si>
-  <si>
-    <t>8c17b9f4-cf40-43f9-b72b-152f0725cf79</t>
-  </si>
-  <si>
-    <t>4755a7ae-84b1-44f6-92dc-d45fe655334e</t>
-  </si>
-  <si>
-    <t>466432a5-d015-46cf-b062-b491055e6ef5</t>
-  </si>
-  <si>
-    <t>45e0cd18-9ec2-4a99-9255-8aa3f5938310</t>
-  </si>
-  <si>
-    <t>5b9a78de-a698-49bb-a2ba-830878f70c5f</t>
-  </si>
-  <si>
-    <t>aa2c8064-6f80-404a-b734-0a496d5021fe</t>
-  </si>
-  <si>
-    <t>a4c7657a-22c5-40b9-a040-0fcbb6627515</t>
-  </si>
-  <si>
-    <t>c3283923-ba01-4ce8-8625-3244a5273564</t>
-  </si>
-  <si>
-    <t>326f8da1-2f12-4d5c-8401-66ba552e86dc</t>
-  </si>
-  <si>
-    <t>b16ea222-6fda-4ea8-b09e-e7cb4b4957a7</t>
-  </si>
-  <si>
-    <t>d1a283ff-7075-447e-a206-4e19c7fac589</t>
-  </si>
-  <si>
-    <t>751d8462-fa4c-471c-827b-4a702cdc4f3b</t>
-  </si>
-  <si>
-    <t>1a1fc05a-1651-45b7-a36f-e003e98fbed6</t>
-  </si>
-  <si>
-    <t>4de0f7f3-0b0f-45f3-a5b3-4ef679713781</t>
-  </si>
-  <si>
-    <t>43b0108c-f14d-4005-9c3d-fd5a2a5d70d2</t>
-  </si>
-  <si>
-    <t>2d675920-5119-4cf8-95fc-3fe3f7a514ad</t>
-  </si>
-  <si>
-    <t>1eec3106-4952-4be1-b215-b30026c30647</t>
-  </si>
-  <si>
-    <t>d9dbef42-bd80-4a79-a749-f1a9009f9ba3</t>
-  </si>
-  <si>
-    <t>cdf62173-75cc-4a80-9503-821602bc224f</t>
-  </si>
-  <si>
-    <t>bef423e0-5aa8-47f0-b143-0042b15954bc</t>
-  </si>
-  <si>
-    <t>48c3b06d-cbfa-49f4-8104-98d809d4baed</t>
-  </si>
-  <si>
-    <t>f2c25422-1ac6-46a9-9ef1-6b6e08289c9c</t>
-  </si>
-  <si>
-    <t>ac24c463-137c-43a2-b491-64f19bb9f98f</t>
-  </si>
-  <si>
-    <t>193b727d-6e79-4d64-8160-a07c0ec6173d</t>
-  </si>
-  <si>
-    <t>66d2775a-c3c6-41d0-9ec5-f3ad8c3171c0</t>
-  </si>
-  <si>
-    <t>c484e5eb-a8a5-4872-ae0a-c00568734153</t>
-  </si>
-  <si>
-    <t>dfb34662-cc9f-437e-b60e-7d66f545d5e7</t>
-  </si>
-  <si>
-    <t>dac00514-c370-4463-b095-37d2106ff60b</t>
-  </si>
-  <si>
-    <t>5e4e7cbf-0f69-4843-8c58-95fdc83fb470</t>
-  </si>
-  <si>
-    <t>4fca153d-119a-4769-9f59-efb41089aefc</t>
-  </si>
-  <si>
-    <t>cfee7538-58b1-457c-b742-94b7dbd5ce09</t>
-  </si>
-  <si>
-    <t>ad86ad1c-5ad0-4730-900f-46255f10062f</t>
-  </si>
-  <si>
-    <t>5ebc086d-24c5-42d1-8bc2-d0c7a872d889</t>
-  </si>
-  <si>
-    <t>8b90128e-2ca8-42f4-9baf-ee4c86594ee9</t>
-  </si>
-  <si>
-    <t>e5af7b8b-8d93-4cd2-8cf9-92220909dadc</t>
-  </si>
-  <si>
-    <t>0dc66570-3ed6-435b-8047-cca3bcb3a7dd</t>
-  </si>
-  <si>
-    <t>131aa5a0-b73c-42c4-8216-1591bf78003f</t>
-  </si>
-  <si>
-    <t>131a8281-825a-4c32-8745-f44cc45d9ee3</t>
-  </si>
-  <si>
-    <t>bc026f13-a32c-46b0-896a-c7190be8510d</t>
-  </si>
-  <si>
-    <t>351cf153-f1b1-40dc-b815-7737514da765</t>
-  </si>
-  <si>
-    <t>1c301312-f68c-4a65-9398-f9e0f569533a</t>
-  </si>
-  <si>
-    <t>5d795434-a4bb-4e6b-8648-e8b8a64ff910</t>
-  </si>
-  <si>
-    <t>a4310bdd-0bdf-4bee-8f9f-ca7cc7137ecf</t>
-  </si>
-  <si>
-    <t>bc018d93-2a9a-460a-af25-7b8aa19b26f8</t>
-  </si>
-  <si>
-    <t>be581463-de77-476b-9d8a-df305d4336f8</t>
-  </si>
-  <si>
-    <t>df80ebe5-9b90-462b-be89-2f07e5a8d4aa</t>
-  </si>
-  <si>
-    <t>3b2463ee-24dd-42d7-a81f-48e21b84d774</t>
-  </si>
-  <si>
-    <t>e1a0dbff-8d5b-429a-8e21-ff5f6a1aa5ca</t>
-  </si>
-  <si>
-    <t>65061c46-4542-4047-a764-c51d66a9df25</t>
-  </si>
-  <si>
-    <t>0c02d348-b698-45ed-b2f0-ff8a17f31a57</t>
-  </si>
-  <si>
-    <t>1e79e36b-39bc-4429-916b-b3c005828157</t>
-  </si>
-  <si>
-    <t>222e6b10-fef6-43ac-931e-93308f2ba189</t>
-  </si>
-  <si>
-    <t>7ed86589-11ec-4cbf-94dd-430d031e1739</t>
-  </si>
-  <si>
-    <t>617e9607-50e7-4793-bab7-14a6614ed62f</t>
-  </si>
-  <si>
-    <t>c1d84020-f811-4aca-ae14-dad1b9ac9b7c</t>
-  </si>
-  <si>
-    <t>c264ff32-eddb-4c1c-b312-4e61a632785c</t>
-  </si>
-  <si>
-    <t>b510bee5-1357-4e41-8cd7-5284df23bd22</t>
-  </si>
-  <si>
-    <t>25133d7a-d26f-4c16-90f1-470089511285</t>
-  </si>
-  <si>
-    <t>7eca1d7c-f347-49d1-bb8f-6155ddb64e99</t>
-  </si>
-  <si>
-    <t>ada5328d-0830-4dcc-8566-8a52933a944c</t>
-  </si>
-  <si>
-    <t>599359d9-1b94-47fa-acd0-8832074849b5</t>
-  </si>
-  <si>
-    <t>2dee2161-3ba2-4a6a-b229-e5f5bebaf0a0</t>
-  </si>
-  <si>
-    <t>ed79a94c-c41e-4d51-85ec-c91b55cff0d6</t>
-  </si>
-  <si>
-    <t>bf06acb4-b334-41b4-9830-e5c0d26ef7db</t>
-  </si>
-  <si>
-    <t>b03a36cb-de29-4a16-8c9e-fd5773e66c46</t>
-  </si>
-  <si>
-    <t>ede831bc-c293-4cac-8f3f-05f5c2e242bc</t>
-  </si>
-  <si>
-    <t>a70c573d-1681-4a27-9d27-2d5770b8148f</t>
-  </si>
-  <si>
-    <t>90f1ca9a-5014-48e7-9b63-01b859f9ec1d</t>
-  </si>
-  <si>
-    <t>757ab6e3-e0e6-4d3a-9117-29725fe4ee45</t>
-  </si>
-  <si>
-    <t>3102402d-78e2-4c1c-8ac7-a58a793a7be4</t>
-  </si>
-  <si>
-    <t>303be9c9-4058-433a-a4ea-a12ca5aaf05a</t>
-  </si>
-  <si>
-    <t>c256e003-c90d-4e98-ae9a-2737f99378c0</t>
-  </si>
-  <si>
-    <t>7736f729-cda8-4076-a454-b629ab7729f6</t>
-  </si>
-  <si>
-    <t>1d1c492d-1202-4387-a972-eea0472ef5e0</t>
-  </si>
-  <si>
-    <t>7fc53743-d27b-4267-8655-ac0df948ca0a</t>
-  </si>
-  <si>
-    <t>679adaf1-ad6f-4555-85fd-fe68d4656de0</t>
-  </si>
-  <si>
-    <t>a70c6c89-bd89-4bcc-9fa8-4c64a395be62</t>
-  </si>
-  <si>
-    <t>5f031783-b4ce-4f91-aaaf-9fa80ebc8cd7</t>
-  </si>
-  <si>
-    <t>d1d8ccb9-2631-4ac3-9d25-d4d1dd41ea9a</t>
-  </si>
-  <si>
-    <t>f8ceb63c-bc09-4ec1-8e7c-0ccce9f92485</t>
-  </si>
-  <si>
-    <t>d09cc870-9dfe-406f-9d8f-d591c34565dc</t>
-  </si>
-  <si>
-    <t>8e39c029-ccea-4ee5-9feb-298c8a10ad9a</t>
-  </si>
-  <si>
-    <t>788f225e-d799-4aad-8042-ab1ea95f7b67</t>
-  </si>
-  <si>
-    <t>c48e4a16-7d8b-492e-b502-ecb005893fb9</t>
-  </si>
-  <si>
-    <t>331c2b0f-c099-45ec-8a9d-127a5cef1feb</t>
-  </si>
-  <si>
-    <t>1a3a8e06-fbae-40ef-95bb-8fd6b0dcc84e</t>
-  </si>
-  <si>
-    <t>0f6f27a1-0eb6-4c85-859d-185823757c06</t>
-  </si>
-  <si>
-    <t>72ba2fda-b00f-43f1-92ad-b6374772d08d</t>
-  </si>
-  <si>
-    <t>27e914de-7bec-42df-9ceb-1be0097e5035</t>
-  </si>
-  <si>
-    <t>7b927f4c-51dd-447c-939f-58430ff45803</t>
-  </si>
-  <si>
-    <t>4e3795db-7131-4448-8262-22a963c3effb</t>
-  </si>
-  <si>
-    <t>18ebe39c-cb63-4f74-87ae-77365ea8e2b1</t>
-  </si>
-  <si>
-    <t>36fce3d9-408f-41bd-842c-cc6afaefad3a</t>
-  </si>
-  <si>
-    <t>45620768-5ebb-42de-8f20-c4404092d274</t>
-  </si>
-  <si>
-    <t>20937843-fac0-4b4e-999a-7bf771d8a744</t>
-  </si>
-  <si>
-    <t>fd378a66-a796-46b3-93f4-81e9a7a16967</t>
-  </si>
-  <si>
-    <t>89b0d0eb-62af-48a9-9079-7b3195aa4164</t>
-  </si>
-  <si>
-    <t>17912e74-264c-4314-a84d-2eb132faab1b</t>
-  </si>
-  <si>
-    <t>49bd41b4-c8b1-4718-90ff-9d38063984f8</t>
-  </si>
-  <si>
-    <t>b2b83e69-7842-403f-8aa4-5376c45c15c2</t>
-  </si>
-  <si>
-    <t>f29c02e5-bc07-415b-9a18-a19282023f29</t>
-  </si>
-  <si>
-    <t>f38c9f06-3fe8-4d28-a736-7e41c1082a86</t>
-  </si>
-  <si>
-    <t>fda29f49-c4b4-4273-b607-89a4d56e7bd1</t>
-  </si>
-  <si>
-    <t>2062f879-327c-48d7-aa41-4b0c0e1d983f</t>
-  </si>
-  <si>
-    <t>01faa3cd-6959-4aae-8641-3a6372c47a71</t>
-  </si>
-  <si>
-    <t>c0c33ae6-fcf7-4f69-a0e7-23b4d5902dae</t>
-  </si>
-  <si>
-    <t>a9113f00-6ca5-444e-832b-4993c9b52b97</t>
-  </si>
-  <si>
-    <t>8b4e256a-1487-4314-835b-408b8b310711</t>
-  </si>
-  <si>
-    <t>248786bc-8c90-4fc5-abb9-4544521b4195</t>
-  </si>
-  <si>
-    <t>90945f3f-2fbd-4725-ae32-235e5d681e10</t>
-  </si>
-  <si>
-    <t>a99172dc-fe1b-42cf-9d8c-49ddc36bec86</t>
-  </si>
-  <si>
-    <t>c91427ec-a335-4359-9394-b3f4a503c2f4</t>
-  </si>
-  <si>
-    <t>57d5f744-6776-4914-859f-985a82eb1314</t>
-  </si>
-  <si>
-    <t>50958680-a5b7-45b1-b7ef-9486658e38cf</t>
-  </si>
-  <si>
-    <t>2492b361-64cd-4e16-bd66-8e6507db507a</t>
-  </si>
-  <si>
-    <t>7a6927dd-1cb3-4abc-8d4d-1446ea1e3967</t>
-  </si>
-  <si>
-    <t>966ca256-8cd8-4078-8751-36fcbdc3381a</t>
-  </si>
-  <si>
-    <t>90fb09df-508d-4c9c-afce-df504abbd757</t>
-  </si>
-  <si>
-    <t>e03cf179-d849-4f29-ac15-c70ca6920a43</t>
-  </si>
-  <si>
-    <t>03f3c131-2875-40fd-bb22-46fa59b88d53</t>
+    <t>eaafa3479e61131a8266b1c3</t>
+  </si>
+  <si>
+    <t>e3174f9a1dd8b82503720670</t>
+  </si>
+  <si>
+    <t>313ecf216036c2ea335999e8</t>
+  </si>
+  <si>
+    <t>bd021be356d3553d759fd460</t>
+  </si>
+  <si>
+    <t>ed384b7bb7b3581f9a5f7cb8</t>
+  </si>
+  <si>
+    <t>8d7b38415c9da8906d998b4b</t>
+  </si>
+  <si>
+    <t>e5e511c7387ea9b754682e21</t>
+  </si>
+  <si>
+    <t>091f4fe03d5155cb806fac7a</t>
+  </si>
+  <si>
+    <t>99849c25f39529e042b1e365</t>
+  </si>
+  <si>
+    <t>1bc454f6cc7ca5b579c61b92</t>
+  </si>
+  <si>
+    <t>6a3d0cb5b8e1a696a9eaafcb</t>
+  </si>
+  <si>
+    <t>a1618adbc9422fe15e00e506</t>
+  </si>
+  <si>
+    <t>d27d768d878aa0a24affb923</t>
+  </si>
+  <si>
+    <t>0a19c769ceb9af107316eeeb</t>
+  </si>
+  <si>
+    <t>ff9a66b461c06f88e8afd02f</t>
+  </si>
+  <si>
+    <t>d3536917b9bca32fcc9ed006</t>
+  </si>
+  <si>
+    <t>4519a6d669e872ba55b0f407</t>
+  </si>
+  <si>
+    <t>9248108086fdf68e07e6c2a3</t>
+  </si>
+  <si>
+    <t>3d633d8b229afd60e6c0a91a</t>
+  </si>
+  <si>
+    <t>08369ef9687cbe73769e8079</t>
+  </si>
+  <si>
+    <t>18ccb13568b4c4f7ea8a9c16</t>
+  </si>
+  <si>
+    <t>df31f01495a12cf1ad344a61</t>
+  </si>
+  <si>
+    <t>37d3b60f2f8a4fdd6bbea4d9</t>
+  </si>
+  <si>
+    <t>24ce3a00888e9933823f3601</t>
+  </si>
+  <si>
+    <t>225c096eca1e1ad3ff0aa079</t>
+  </si>
+  <si>
+    <t>d16bdb30b9a3638db5d05290</t>
+  </si>
+  <si>
+    <t>9f7234034c6a97191176829e</t>
+  </si>
+  <si>
+    <t>aaaf69dbb3c0877e6ed00feb</t>
+  </si>
+  <si>
+    <t>e6e62662acc99702b736aab2</t>
+  </si>
+  <si>
+    <t>e3b4d1a15b9cb74649cb7367</t>
+  </si>
+  <si>
+    <t>ce4006beb10fa8b80ee9c189</t>
+  </si>
+  <si>
+    <t>491823f5a62cc3eb4cd2979b</t>
+  </si>
+  <si>
+    <t>fda1b26479655b051c9e19c5</t>
+  </si>
+  <si>
+    <t>f2b4ea77828144851a9e813c</t>
+  </si>
+  <si>
+    <t>303ef116e17afa6b13581fcd</t>
+  </si>
+  <si>
+    <t>bacc4cc7e2df2f78ab697721</t>
+  </si>
+  <si>
+    <t>d91ed52bbbcbc9e6496bf9e5</t>
+  </si>
+  <si>
+    <t>502d5ac0e0753d3705cec6bc</t>
+  </si>
+  <si>
+    <t>7845f376d4650ec8b8c2d495</t>
+  </si>
+  <si>
+    <t>2484ab03f167b56e6c6c52e2</t>
+  </si>
+  <si>
+    <t>ea51496526d5acd13b6a4c21</t>
+  </si>
+  <si>
+    <t>3c5612fa5eb17d4139ac5eb2</t>
+  </si>
+  <si>
+    <t>892107e09835f8407127c2c0</t>
+  </si>
+  <si>
+    <t>602dec82448c8e67843399ae</t>
+  </si>
+  <si>
+    <t>e6f4f47fb7bbd3b0da04941a</t>
+  </si>
+  <si>
+    <t>2c3ede3e52f600bf3ade8131</t>
+  </si>
+  <si>
+    <t>9ee900030391d5552575e101</t>
+  </si>
+  <si>
+    <t>dd340bf96de5541deb9348a6</t>
+  </si>
+  <si>
+    <t>3b2baae591f9cd3a2eb8407f</t>
+  </si>
+  <si>
+    <t>5c3c3a43f161a72509949b2b</t>
+  </si>
+  <si>
+    <t>bb7a50b9ae355c5c6b8eaf01</t>
+  </si>
+  <si>
+    <t>f90663e2d059e44a62be373e</t>
+  </si>
+  <si>
+    <t>bce06298c9b13326406cc744</t>
+  </si>
+  <si>
+    <t>37e587d1a2367892fe21614f</t>
+  </si>
+  <si>
+    <t>42207b9f943820b8a5f5d545</t>
+  </si>
+  <si>
+    <t>f656eb05ce8d9fff366aa95c</t>
+  </si>
+  <si>
+    <t>61a0315baefc4125bfefd6fb</t>
+  </si>
+  <si>
+    <t>5025ebaec80fd9f3e1fa559f</t>
+  </si>
+  <si>
+    <t>c648424576426937a679945a</t>
+  </si>
+  <si>
+    <t>267d80cd3b50877f1be2bb64</t>
+  </si>
+  <si>
+    <t>6bf7488cc8851c9fb82796f2</t>
+  </si>
+  <si>
+    <t>b6af6eb2a487322ea12f4790</t>
+  </si>
+  <si>
+    <t>e1ca41514d830f05d23dcf29</t>
+  </si>
+  <si>
+    <t>1b9c4b761a195a020f940ce2</t>
+  </si>
+  <si>
+    <t>e8bccb09cc4c24ea92d24389</t>
+  </si>
+  <si>
+    <t>c507afd75e0621974d6a865e</t>
+  </si>
+  <si>
+    <t>abf06d83e037bf455cf80ce0</t>
+  </si>
+  <si>
+    <t>e0d74a7a8b7ccfbe7fa09335</t>
+  </si>
+  <si>
+    <t>b599b33872da2b8aeed5e390</t>
+  </si>
+  <si>
+    <t>4e60d3cce300b1db14126f2d</t>
+  </si>
+  <si>
+    <t>5ff01de55dc4f7f87816b3a2</t>
+  </si>
+  <si>
+    <t>e1e69eed22f33eb833ae5123</t>
+  </si>
+  <si>
+    <t>f4edeb6b1f63ea9943cf1e9d</t>
+  </si>
+  <si>
+    <t>1fcf5ab51cc6cfde10b24ff1</t>
+  </si>
+  <si>
+    <t>0ce7f030414c4e5fd856c787</t>
+  </si>
+  <si>
+    <t>6e24434334445394267d108c</t>
+  </si>
+  <si>
+    <t>006bf4947b5e8874c904c0d6</t>
+  </si>
+  <si>
+    <t>c044dcf7fce431e29e78a2f6</t>
+  </si>
+  <si>
+    <t>649ab97880e9de15842701f4</t>
+  </si>
+  <si>
+    <t>23f1538730082b030760efc3</t>
+  </si>
+  <si>
+    <t>52c9b39340825fdca855a338</t>
+  </si>
+  <si>
+    <t>f8853fb57caad034abf68250</t>
+  </si>
+  <si>
+    <t>7571e135258ab68a378c49f3</t>
+  </si>
+  <si>
+    <t>8de8f6ff211fbf6b75b44fea</t>
+  </si>
+  <si>
+    <t>9f1e8a3439a38fafe0c02140</t>
+  </si>
+  <si>
+    <t>e6a7f05b8aaca7fe28e52e6d</t>
+  </si>
+  <si>
+    <t>15614b575610a9dd63d93f41</t>
+  </si>
+  <si>
+    <t>2b201e9ec4af0e270fab95ee</t>
+  </si>
+  <si>
+    <t>c64fd0af468e8e425eaed448</t>
+  </si>
+  <si>
+    <t>a0ff348f9bf1f27b7da2a068</t>
+  </si>
+  <si>
+    <t>f0839b9a1a7c6a857df52e90</t>
+  </si>
+  <si>
+    <t>356589e84219d607097a522d</t>
+  </si>
+  <si>
+    <t>73df12e1d7458c1c70ca2618</t>
+  </si>
+  <si>
+    <t>73a216e96bc7263be7574dbf</t>
+  </si>
+  <si>
+    <t>335e8f242757e2a033af6d66</t>
+  </si>
+  <si>
+    <t>f1cfaa8bb082b8014c346547</t>
+  </si>
+  <si>
+    <t>73e43b557b2a38a68bebf63d</t>
+  </si>
+  <si>
+    <t>ee0c598fc71703e7eb3162a3</t>
+  </si>
+  <si>
+    <t>50cb7d8c03d83d44c7de025f</t>
+  </si>
+  <si>
+    <t>034c7a242e52eac708b6651b</t>
+  </si>
+  <si>
+    <t>bf10027906d9d6f1f2a29e88</t>
+  </si>
+  <si>
+    <t>9965bf262fe5e30b702514e1</t>
+  </si>
+  <si>
+    <t>5229148f81ad3f9d9ea5be2c</t>
+  </si>
+  <si>
+    <t>5c3418d927e8baec7e47cea8</t>
+  </si>
+  <si>
+    <t>2298a3e4701e9f0d60f3277d</t>
+  </si>
+  <si>
+    <t>1228bc74395f9a31603bc885</t>
+  </si>
+  <si>
+    <t>f143bda0a86e8c9f1ebf41f8</t>
+  </si>
+  <si>
+    <t>7803055c8a22308dfb0553a0</t>
+  </si>
+  <si>
+    <t>dd96e7550053a1d9535bc5dc</t>
+  </si>
+  <si>
+    <t>c0d25c157184d69b6cdb4a0f</t>
+  </si>
+  <si>
+    <t>b5c872f33e784e699ec775f4</t>
+  </si>
+  <si>
+    <t>530985c92e417e09c2394ee5</t>
+  </si>
+  <si>
+    <t>2a8545c3dee837174ee74197</t>
+  </si>
+  <si>
+    <t>7233f8dddc83f109f150eda0</t>
+  </si>
+  <si>
+    <t>200865dc1284cc1c6d44f1fa</t>
+  </si>
+  <si>
+    <t>3010d5b3f4df9de4c1c15633</t>
+  </si>
+  <si>
+    <t>26fe143555e639daed8a07cb</t>
+  </si>
+  <si>
+    <t>53519a4599d71daf7202789d</t>
+  </si>
+  <si>
+    <t>e35a72a7525ab96b7bd80c59</t>
+  </si>
+  <si>
+    <t>08a7d194a804191244a64ac6</t>
+  </si>
+  <si>
+    <t>2bd2ebfabb987955a729f9ed</t>
+  </si>
+  <si>
+    <t>98c5c8f472724521d0d85682</t>
+  </si>
+  <si>
+    <t>8c91c9ee3ac825d369430fc5</t>
+  </si>
+  <si>
+    <t>31cc5900dcfd27c411c7965e</t>
+  </si>
+  <si>
+    <t>a74b4d829d15f78814e0fb24</t>
+  </si>
+  <si>
+    <t>047e024528b89b2e99b61418</t>
+  </si>
+  <si>
+    <t>ef35098445ebaf32ef39cb96</t>
+  </si>
+  <si>
+    <t>a0470faa0feff29254472b54</t>
+  </si>
+  <si>
+    <t>6f4a987f0cca26daaea28652</t>
+  </si>
+  <si>
+    <t>1668bcc5d334b4b453671fce</t>
+  </si>
+  <si>
+    <t>6b5bc4794ec3ab466f8ffc71</t>
+  </si>
+  <si>
+    <t>585c716714528d911f4e3149</t>
+  </si>
+  <si>
+    <t>7d0cae88929d4a2a9a5933f9</t>
+  </si>
+  <si>
+    <t>fd518f380b1a336de82413f1</t>
+  </si>
+  <si>
+    <t>a7ae35fd1f6588c1255548c9</t>
+  </si>
+  <si>
+    <t>8bd951f77348399f5c997ac1</t>
+  </si>
+  <si>
+    <t>72dfc34b266df9015bf3d811</t>
+  </si>
+  <si>
+    <t>271df53ad5a9bb1659d921d5</t>
+  </si>
+  <si>
+    <t>91eeee7f87c8df8229dfcbed</t>
+  </si>
+  <si>
+    <t>9d8b254b87beedc0f8ceee9c</t>
+  </si>
+  <si>
+    <t>150c9cef6d8c677d4da265b5</t>
+  </si>
+  <si>
+    <t>bda431e980226bb259ae5aca</t>
+  </si>
+  <si>
+    <t>e0cdccb71c9597618b90397c</t>
+  </si>
+  <si>
+    <t>ad0d5f496712922904a5a3ec</t>
+  </si>
+  <si>
+    <t>e398b7709179028fc366913e</t>
+  </si>
+  <si>
+    <t>985bbd27aa4c2b267e05464b</t>
+  </si>
+  <si>
+    <t>2f915fb8aee0569efd25c4d6</t>
+  </si>
+  <si>
+    <t>218bdd61ba62b372003cf130</t>
+  </si>
+  <si>
+    <t>2f9ea9f0979de9168ee06807</t>
+  </si>
+  <si>
+    <t>bf17ed869e36f6cb4703f8e5</t>
+  </si>
+  <si>
+    <t>0d03bc1c80f05357d11688e8</t>
+  </si>
+  <si>
+    <t>b8160ddd92f757d4e7a46110</t>
+  </si>
+  <si>
+    <t>5e1f17fe123bafc1291f844d</t>
+  </si>
+  <si>
+    <t>d98fb0dd01dbe2d10df84767</t>
+  </si>
+  <si>
+    <t>f7f6d048d02e4f2112fd7dcc</t>
+  </si>
+  <si>
+    <t>9ac0b267400cf80f7e501158</t>
+  </si>
+  <si>
+    <t>6630ef2ce5e748376a012f37</t>
+  </si>
+  <si>
+    <t>50d31232729ed17b16ddfc00</t>
+  </si>
+  <si>
+    <t>9b106f709d373334e0527d4a</t>
+  </si>
+  <si>
+    <t>55d3e14bfc73ed3f5c9ad67d</t>
+  </si>
+  <si>
+    <t>b9375e4a74a63c14fc0d70d7</t>
+  </si>
+  <si>
+    <t>9ec55b5cefa14bd55c161979</t>
+  </si>
+  <si>
+    <t>5ad7a4b17998839bdf3981e0</t>
+  </si>
+  <si>
+    <t>d3c703c0d17bff67b97db6f9</t>
+  </si>
+  <si>
+    <t>b3923d73a5015add121cdb43</t>
+  </si>
+  <si>
+    <t>d6a0ac7c0c51ce89f0897ae8</t>
+  </si>
+  <si>
+    <t>f77d5306e84fa0cc33669041</t>
+  </si>
+  <si>
+    <t>34469e67dc58eeb6ac5d4f6e</t>
+  </si>
+  <si>
+    <t>c0ea65c76e8a012296700954</t>
+  </si>
+  <si>
+    <t>50fb671cadf2e23feaf9b6c2</t>
+  </si>
+  <si>
+    <t>5fb8a31653e0d1417a6f69d6</t>
+  </si>
+  <si>
+    <t>fbc748b5c3c3c4909f010aed</t>
+  </si>
+  <si>
+    <t>4ad5235559d315f35cdd9ddc</t>
+  </si>
+  <si>
+    <t>b3a39ad674d23fb3706239ef</t>
+  </si>
+  <si>
+    <t>04282eb470189d982c139c01</t>
+  </si>
+  <si>
+    <t>4e6b364b6937f934d79b9b22</t>
+  </si>
+  <si>
+    <t>16fff09a377ced60c96d1cc2</t>
+  </si>
+  <si>
+    <t>528611f1636f1605dbafca70</t>
+  </si>
+  <si>
+    <t>663145f448917d29d3add506</t>
+  </si>
+  <si>
+    <t>d60d63e3b4e6ecfdc2f2b23a</t>
+  </si>
+  <si>
+    <t>60ab5084c645fa86bd386b2c</t>
+  </si>
+  <si>
+    <t>cb58fdc885f81e01c5132ced</t>
+  </si>
+  <si>
+    <t>0f6275944cda61bfcebd7fa7</t>
+  </si>
+  <si>
+    <t>baacba1f3a3ae8d935dccbfe</t>
+  </si>
+  <si>
+    <t>5b7257806676b6e3e14c601b</t>
+  </si>
+  <si>
+    <t>eef36864a95ed44b2bd74eb0</t>
+  </si>
+  <si>
+    <t>02cb7412c55de81597b0ab0d</t>
+  </si>
+  <si>
+    <t>63028c97c45005c83488ae6c</t>
+  </si>
+  <si>
+    <t>b4b6d26d0619376e6de3e628</t>
+  </si>
+  <si>
+    <t>07ce292079794c0bc59ce05d</t>
+  </si>
+  <si>
+    <t>2772d7ce81fef98846241e41</t>
+  </si>
+  <si>
+    <t>0893e2b464d033f04d0a870b</t>
+  </si>
+  <si>
+    <t>8ff20989e75cb5a7a80bcd82</t>
+  </si>
+  <si>
+    <t>78fd678c191fa166694a2c04</t>
+  </si>
+  <si>
+    <t>9e575cffd9f04878d6ae3204</t>
+  </si>
+  <si>
+    <t>4422272dae4187c454f335a2</t>
+  </si>
+  <si>
+    <t>9e0b503f3c17b0e3339bfca4</t>
+  </si>
+  <si>
+    <t>b09b7eaf4171812d41c0fb5b</t>
+  </si>
+  <si>
+    <t>7b3e51e19434385c4f0a7625</t>
+  </si>
+  <si>
+    <t>39f9f94d49c5cd021b40e892</t>
+  </si>
+  <si>
+    <t>0c0d3242f27af5609dbd50e8</t>
+  </si>
+  <si>
+    <t>565adb5d0c6e89f259dbb299</t>
+  </si>
+  <si>
+    <t>eb1fee37c5ab0adee1a7495c</t>
+  </si>
+  <si>
+    <t>1bf0c8728c3bb3e7437e506c</t>
+  </si>
+  <si>
+    <t>58048db16a0dce12014de1f9</t>
+  </si>
+  <si>
+    <t>6dcd918acec64a7c238236b1</t>
+  </si>
+  <si>
+    <t>1b5f04f183dd3633654a8a63</t>
+  </si>
+  <si>
+    <t>89ef5dc5e0f7501514968994</t>
+  </si>
+  <si>
+    <t>fda59bc29c057545ba26da47</t>
+  </si>
+  <si>
+    <t>eeaad1a2368e631f83f161a4</t>
+  </si>
+  <si>
+    <t>045174131de8b9f9ecba7d5c</t>
+  </si>
+  <si>
+    <t>39fabc9a14505362b93b07a7</t>
+  </si>
+  <si>
+    <t>18b239b148e011f1dc7f8a26</t>
+  </si>
+  <si>
+    <t>bd55164e425d33c201b45dd8</t>
+  </si>
+  <si>
+    <t>c90b8f55a46daade2345a34c</t>
+  </si>
+  <si>
+    <t>353b7849dec51213881fc2f5</t>
+  </si>
+  <si>
+    <t>86bbffced836349d5fbaa0ab</t>
+  </si>
+  <si>
+    <t>9c8b11aad095c3c3580b1d34</t>
+  </si>
+  <si>
+    <t>225df6269d7fdcedbea38280</t>
+  </si>
+  <si>
+    <t>a992388b3c3381148fb12518</t>
+  </si>
+  <si>
+    <t>69dcdee0a6dfd2130f36c953</t>
+  </si>
+  <si>
+    <t>b457de7c7c6dc391106b1dd9</t>
+  </si>
+  <si>
+    <t>e87786454bcb96dcc81dc4c7</t>
+  </si>
+  <si>
+    <t>eb2a9948563b0575a1ce02c7</t>
+  </si>
+  <si>
+    <t>d5cfe3127d61dfda9694baa9</t>
+  </si>
+  <si>
+    <t>db9fae33b478e2881fdb8bfc</t>
+  </si>
+  <si>
+    <t>c935bc31757423b3ffbc0162</t>
+  </si>
+  <si>
+    <t>af1fc3462249ef206cdfd9c9</t>
+  </si>
+  <si>
+    <t>bbf40ff7cb5e1577e41ec951</t>
+  </si>
+  <si>
+    <t>841da509dd68126162432a5a</t>
+  </si>
+  <si>
+    <t>e16a2c43cbb934b25533d483</t>
+  </si>
+  <si>
+    <t>a912fee09f3bb0043765dd3c</t>
+  </si>
+  <si>
+    <t>350043f49215da070cc89de9</t>
+  </si>
+  <si>
+    <t>82f2121aa79d53795e5e0eab</t>
+  </si>
+  <si>
+    <t>63b7b8ead909b4d6ed761c8a</t>
+  </si>
+  <si>
+    <t>5222d4525d872f17c63d07f4</t>
+  </si>
+  <si>
+    <t>d9a48ae43d496afe61618cc9</t>
+  </si>
+  <si>
+    <t>302e962fb0804514f9251094</t>
+  </si>
+  <si>
+    <t>f99e91007cb94aa54a91118e</t>
+  </si>
+  <si>
+    <t>321df605d9bd308e1224cf53</t>
+  </si>
+  <si>
+    <t>108fc9f407eebeeb6e637e5d</t>
+  </si>
+  <si>
+    <t>9f91d81dfb50cd2bcca32cb5</t>
+  </si>
+  <si>
+    <t>863b60918ed4d010f70029c8</t>
+  </si>
+  <si>
+    <t>105b8d27a0562d1c74a55001</t>
+  </si>
+  <si>
+    <t>8af2315d5e0b258bf404e023</t>
+  </si>
+  <si>
+    <t>c108e25ce4457c3bf372a51b</t>
+  </si>
+  <si>
+    <t>203de79d248cc57d979c7bfa</t>
+  </si>
+  <si>
+    <t>d3bbefbe22b9863ae0a61ab4</t>
+  </si>
+  <si>
+    <t>74f641bf1681fe6c6daf4650</t>
+  </si>
+  <si>
+    <t>910f7e38b4249eb924ec4757</t>
+  </si>
+  <si>
+    <t>833f9cec4dc2ca81639f7add</t>
+  </si>
+  <si>
+    <t>1ef55a1b18ab7372aee7a079</t>
+  </si>
+  <si>
+    <t>d2023c1fa5346af6541d766d</t>
+  </si>
+  <si>
+    <t>3836f3f5c03fefc861007be7</t>
+  </si>
+  <si>
+    <t>74200772832a3ef54cf36cd6</t>
+  </si>
+  <si>
+    <t>638c40c7a471fe04983c09be</t>
+  </si>
+  <si>
+    <t>7983438e2547d71939e0d4e7</t>
+  </si>
+  <si>
+    <t>f517188f727d195d0c19f6ca</t>
+  </si>
+  <si>
+    <t>d262354788cb568295a24d62</t>
+  </si>
+  <si>
+    <t>c5a7f4372db9bc14419f98ff</t>
+  </si>
+  <si>
+    <t>4bae40bcdb4f3b6bb4c638e2</t>
+  </si>
+  <si>
+    <t>eeb73997365f4796fa1ef11f</t>
+  </si>
+  <si>
+    <t>47c1180ec52942fa3f1bb95a</t>
+  </si>
+  <si>
+    <t>31dc4726661d4835ea635735</t>
+  </si>
+  <si>
+    <t>ee1d7c03961e8c7b3eb25923</t>
+  </si>
+  <si>
+    <t>d61050ae92702859bfa9b517</t>
+  </si>
+  <si>
+    <t>747c23775fe96b729dcb02bb</t>
+  </si>
+  <si>
+    <t>4a8db21005a77ad38d7b1529</t>
+  </si>
+  <si>
+    <t>11805f1246c98d52978726dc</t>
+  </si>
+  <si>
+    <t>2ce785e1fd8e744298737329</t>
+  </si>
+  <si>
+    <t>994dd803511b54a445ae42f8</t>
+  </si>
+  <si>
+    <t>5e3daabd157be2afaf88f209</t>
+  </si>
+  <si>
+    <t>8af1d858b6dacc6052c022a2</t>
+  </si>
+  <si>
+    <t>e5c12cfaafdc0e2a6ed72232</t>
+  </si>
+  <si>
+    <t>f821270d3d62b3879f14050e</t>
+  </si>
+  <si>
+    <t>2cc7e03eaf4e19ef3e2f7b19</t>
+  </si>
+  <si>
+    <t>4ecc316f1441cbc4fb8f164a</t>
+  </si>
+  <si>
+    <t>4510d4d618128104deae1a53</t>
+  </si>
+  <si>
+    <t>767cbdc975dc0fd7639b0643</t>
+  </si>
+  <si>
+    <t>010d951958c104a144a954e8</t>
+  </si>
+  <si>
+    <t>8381f44c019491948e22a280</t>
+  </si>
+  <si>
+    <t>bbfdcbdf5d510265ebe8ef37</t>
+  </si>
+  <si>
+    <t>d6b89b6d0b79cfab58b1d626</t>
+  </si>
+  <si>
+    <t>e2382338b604daf4bae3a0a2</t>
+  </si>
+  <si>
+    <t>1f53f90cb067830f6b86bae1</t>
+  </si>
+  <si>
+    <t>5ad86684dd92b5c33f7668f9</t>
+  </si>
+  <si>
+    <t>1d4f7d01a40fe9deb0734533</t>
+  </si>
+  <si>
+    <t>a1e3510d07cec3600038979b</t>
+  </si>
+  <si>
+    <t>3137a7c38a3d2b54a71c1db6</t>
+  </si>
+  <si>
+    <t>10fe873a0e1a4ba7305b0dfb</t>
+  </si>
+  <si>
+    <t>9b4700c2e8858507f31c330a</t>
+  </si>
+  <si>
+    <t>2c7d221a8b506983ee9c5057</t>
+  </si>
+  <si>
+    <t>9e1b43934cbe15420e202f94</t>
+  </si>
+  <si>
+    <t>0f2693bbb793555be2b42221</t>
+  </si>
+  <si>
+    <t>69da376d9b42614519b23e44</t>
+  </si>
+  <si>
+    <t>50cf2a0176f78c808059e55f</t>
+  </si>
+  <si>
+    <t>5aa5a7e7005c2ab1de6093cf</t>
+  </si>
+  <si>
+    <t>0b9701dc084f3c856da0dce2</t>
+  </si>
+  <si>
+    <t>38a1e86e0372e01340949e02</t>
+  </si>
+  <si>
+    <t>70c2517c5fe14cab0683634d</t>
+  </si>
+  <si>
+    <t>e132770e375eed83913faf3e</t>
+  </si>
+  <si>
+    <t>ddf8c739b04b7242cc6234ff</t>
+  </si>
+  <si>
+    <t>49196e4e35bdd38ae0fa3841</t>
+  </si>
+  <si>
+    <t>edf654f7f91e7a094dc1aba4</t>
+  </si>
+  <si>
+    <t>aa5be902cab7b378d54f37e0</t>
+  </si>
+  <si>
+    <t>31deb8c125d4d4bab7b8b02a</t>
+  </si>
+  <si>
+    <t>743fda8a0089befc7aaaa175</t>
+  </si>
+  <si>
+    <t>5c7660253bbc809a944d679a</t>
+  </si>
+  <si>
+    <t>fd2b322c0889ab271be4443d</t>
+  </si>
+  <si>
+    <t>3832949419271c761c074053</t>
+  </si>
+  <si>
+    <t>1075b7b985c7a51194acdbd3</t>
+  </si>
+  <si>
+    <t>f6f03062f1600aef3163a4e0</t>
+  </si>
+  <si>
+    <t>764d284bcfd90651357d1869</t>
+  </si>
+  <si>
+    <t>a26fa2f5a62efb523c644bfc</t>
+  </si>
+  <si>
+    <t>c226b8695121e18b8f0874df</t>
+  </si>
+  <si>
+    <t>8f71435eb5c72dcf94c7154a</t>
+  </si>
+  <si>
+    <t>f47acceb5d0ebfa01b1480ed</t>
+  </si>
+  <si>
+    <t>c5673aaeaac66068928cbc34</t>
+  </si>
+  <si>
+    <t>190951a1bd3b31d844037f97</t>
+  </si>
+  <si>
+    <t>92158cad27f2ba5f520d9f73</t>
+  </si>
+  <si>
+    <t>ed42328e27820c70787995b8</t>
+  </si>
+  <si>
+    <t>b2955c4ade76316dc256947f</t>
+  </si>
+  <si>
+    <t>b079b90c480d3f3a25a1c3c7</t>
+  </si>
+  <si>
+    <t>d8a8a09938e2bd5d1472e7ca</t>
+  </si>
+  <si>
+    <t>1b3a03b494c7f1eea5a3844f</t>
+  </si>
+  <si>
+    <t>cb3b8b60d77998b42f959f6c</t>
+  </si>
+  <si>
+    <t>f1d0e2d37f45de0a873c9539</t>
+  </si>
+  <si>
+    <t>f29ea98f0cb2829297684c91</t>
+  </si>
+  <si>
+    <t>9225517d16581ee8390a48dd</t>
+  </si>
+  <si>
+    <t>b99d5fb90505db32d4ac41a1</t>
+  </si>
+  <si>
+    <t>6100457614426715316d089c</t>
+  </si>
+  <si>
+    <t>5e528df011fb068528d11704</t>
+  </si>
+  <si>
+    <t>d5838ed73e58fc1753b0f324</t>
+  </si>
+  <si>
+    <t>f387ba3da9964e2ac8800a5e</t>
+  </si>
+  <si>
+    <t>da1fa28b0e8ed1ebece2ddf6</t>
+  </si>
+  <si>
+    <t>9aadaa6e457626a1a00e3ad3</t>
+  </si>
+  <si>
+    <t>710ec6793c3bb3ca2d1de416</t>
+  </si>
+  <si>
+    <t>60c426c1d76d62e3ac37df29</t>
+  </si>
+  <si>
+    <t>9b5ec11ca2b41eca65d2b127</t>
+  </si>
+  <si>
+    <t>06de8104cfc03efac06ab7a5</t>
+  </si>
+  <si>
+    <t>97aee897b5b5da80264682e1</t>
+  </si>
+  <si>
+    <t>4a4e51f598ef58484f983ad7</t>
+  </si>
+  <si>
+    <t>fc5aa563ae4fbbeb1ad30f7a</t>
+  </si>
+  <si>
+    <t>1ae465b2b23c87258b82cda1</t>
+  </si>
+  <si>
+    <t>739aef80609cc8dc9d500727</t>
+  </si>
+  <si>
+    <t>5f3f344ced62aaad0cf6e873</t>
+  </si>
+  <si>
+    <t>6f6cc6381e37d1c2898c7b81</t>
+  </si>
+  <si>
+    <t>ad001e1336afbab83f3c2726</t>
+  </si>
+  <si>
+    <t>ed805f68804c534983d40633</t>
+  </si>
+  <si>
+    <t>4e3a900e3f18cefd48609bf6</t>
+  </si>
+  <si>
+    <t>eb16fffd3573085a49a0ca3a</t>
+  </si>
+  <si>
+    <t>cf6542d10328826df00ebaa3</t>
+  </si>
+  <si>
+    <t>1dade9ab3aee4390897cb273</t>
+  </si>
+  <si>
+    <t>5974e9d719a6844802db308f</t>
+  </si>
+  <si>
+    <t>0140f78c8a78c2c60c0bb82c</t>
+  </si>
+  <si>
+    <t>b4e5c076ff6f59590513d7ea</t>
+  </si>
+  <si>
+    <t>d2bcfa185c2e235dfb91f600</t>
+  </si>
+  <si>
+    <t>fae0105a915132cda22dea67</t>
+  </si>
+  <si>
+    <t>831dd8d117b7536558363df0</t>
+  </si>
+  <si>
+    <t>ed87b9a8e5d56ccb825cf019</t>
+  </si>
+  <si>
+    <t>de864d71e4afd3b95c3cd65b</t>
+  </si>
+  <si>
+    <t>fc900346d46343bc4a4a776a</t>
+  </si>
+  <si>
+    <t>dd146b2b1c1f273f65d7fb9f</t>
+  </si>
+  <si>
+    <t>bd7ee35b45c5b471e73db3ca</t>
+  </si>
+  <si>
+    <t>9c36d6f3eac16f931bb37e42</t>
+  </si>
+  <si>
+    <t>aebfd693bf031f559dc5949a</t>
+  </si>
+  <si>
+    <t>6acedcf32324fd119a6073e5</t>
+  </si>
+  <si>
+    <t>14f5c2a2dcdb609f07af9ba3</t>
+  </si>
+  <si>
+    <t>17827e9d74581d535d120a60</t>
+  </si>
+  <si>
+    <t>30d0fdeaaa11fca81b9cc991</t>
+  </si>
+  <si>
+    <t>a69cf4e47dbc9f5fe1f887b4</t>
+  </si>
+  <si>
+    <t>89b2e5213ce7d361e2d44cb6</t>
+  </si>
+  <si>
+    <t>082d134dc3d5ec08eab8eeec</t>
+  </si>
+  <si>
+    <t>ec71f30f70c7c8b51315622f</t>
+  </si>
+  <si>
+    <t>ea8b883a0cd07e00f0363ec2</t>
+  </si>
+  <si>
+    <t>9295bfb4e6df99f33835031f</t>
+  </si>
+  <si>
+    <t>61daac55e78142735c9d9367</t>
+  </si>
+  <si>
+    <t>77e04df9817135daf552a8e4</t>
+  </si>
+  <si>
+    <t>2eb0c7200bfc816d7319b6ee</t>
+  </si>
+  <si>
+    <t>57bfc37acf48534820963c32</t>
+  </si>
+  <si>
+    <t>f423373972122cbd06844f54</t>
+  </si>
+  <si>
+    <t>ae831e8d18eecc85364eacba</t>
+  </si>
+  <si>
+    <t>0dd9643d24c71a6fd2d3626e</t>
+  </si>
+  <si>
+    <t>04bf9be4544e22e90358bbcc</t>
+  </si>
+  <si>
+    <t>4a60e771f122ab6b9ae478fd</t>
+  </si>
+  <si>
+    <t>f3d9785b54db00569b5d4325</t>
+  </si>
+  <si>
+    <t>ed9b2c9a588db95d2409be8e</t>
+  </si>
+  <si>
+    <t>409e8e8a2e88869ebc2d983a</t>
+  </si>
+  <si>
+    <t>545e8c5ac718b67a17930e9f</t>
+  </si>
+  <si>
+    <t>b695d2d93b5af475fb90248b</t>
+  </si>
+  <si>
+    <t>4f663e775ac43e71bc9df0fc</t>
+  </si>
+  <si>
+    <t>9f87e5989c4df42dc4b1ad3e</t>
+  </si>
+  <si>
+    <t>cebfe6fcdc244b4403b4e193</t>
+  </si>
+  <si>
+    <t>aafd524fedead81d850d955b</t>
+  </si>
+  <si>
+    <t>d881ff71ba76331b50807d57</t>
+  </si>
+  <si>
+    <t>07602f36d0c38e4d22a78076</t>
+  </si>
+  <si>
+    <t>bdaac92e86bbb93134fb538f</t>
+  </si>
+  <si>
+    <t>8b1e6649e35ba19b35b9dd25</t>
+  </si>
+  <si>
+    <t>9a251708b2a71487c053cfff</t>
+  </si>
+  <si>
+    <t>8bf0973f4efb88f3cc182c21</t>
+  </si>
+  <si>
+    <t>2aa90cfce4167b6da206b881</t>
+  </si>
+  <si>
+    <t>97d1bac27e9b4aa49cebeb6b</t>
+  </si>
+  <si>
+    <t>73d6041f2a9f78da324405d5</t>
+  </si>
+  <si>
+    <t>357cbf202b5fe56e762a90cf</t>
+  </si>
+  <si>
+    <t>eb3faa92364b470025ce1578</t>
+  </si>
+  <si>
+    <t>ff15ef3e7054160b17104f87</t>
+  </si>
+  <si>
+    <t>d237c984a8225e9b84e92f5e</t>
+  </si>
+  <si>
+    <t>a981acfe2b8d8dbb6a222984</t>
+  </si>
+  <si>
+    <t>278ec80be6a25001585f7873</t>
+  </si>
+  <si>
+    <t>34c19112aae500dd6e99acd0</t>
+  </si>
+  <si>
+    <t>1038e5eee07de90aa81b925d</t>
+  </si>
+  <si>
+    <t>29effb0c46ca493210d0f044</t>
+  </si>
+  <si>
+    <t>cfe58090d25889845b0c64f4</t>
+  </si>
+  <si>
+    <t>ab2afcac931a3358d08a58b0</t>
+  </si>
+  <si>
+    <t>5feab88a954b353ed52d960c</t>
+  </si>
+  <si>
+    <t>feca25e5e386cd6e58c9f173</t>
+  </si>
+  <si>
+    <t>34c4b6f4a6e45405328fe2b4</t>
+  </si>
+  <si>
+    <t>4676a036a48bc9a44bde308c</t>
+  </si>
+  <si>
+    <t>d1b7477e89e6bc7ea02abba2</t>
+  </si>
+  <si>
+    <t>3b9c4380125b22ab20d6dece</t>
+  </si>
+  <si>
+    <t>edfbea85fd9a5c6fb00ac74b</t>
+  </si>
+  <si>
+    <t>74a6b0cbb1dd2515331253d3</t>
+  </si>
+  <si>
+    <t>2f1c908e083f33e1058256fa</t>
+  </si>
+  <si>
+    <t>94f0b8d4edcba3ffbcbb6908</t>
+  </si>
+  <si>
+    <t>06d0787f76009203b491cf99</t>
+  </si>
+  <si>
+    <t>79050d7b6660a5bd93661f2d</t>
+  </si>
+  <si>
+    <t>91c570b73ab10d2736a5c3ed</t>
+  </si>
+  <si>
+    <t>e91c5d29bec18b3b5bcfddb4</t>
+  </si>
+  <si>
+    <t>d0a110c36598450669b2b1e4</t>
+  </si>
+  <si>
+    <t>883db8d860b16f181471489f</t>
+  </si>
+  <si>
+    <t>9e3836740b574fb2bf41a241</t>
+  </si>
+  <si>
+    <t>f2f37f86c4be7ca5444f3590</t>
+  </si>
+  <si>
+    <t>cb8b03ae3d6baa9dfcc5b803</t>
+  </si>
+  <si>
+    <t>d49eee6a981a748e4253de11</t>
+  </si>
+  <si>
+    <t>1c0b683dae4ed41cd6518bdd</t>
+  </si>
+  <si>
+    <t>f563f1d54a585f78164008f4</t>
+  </si>
+  <si>
+    <t>f8cf980e6a62667ebbe240c9</t>
+  </si>
+  <si>
+    <t>3f47e77c867c644fb1d4b4b6</t>
+  </si>
+  <si>
+    <t>508b4935912bb84eaee637a1</t>
+  </si>
+  <si>
+    <t>9c5073f0a2b50034fe41ea3e</t>
+  </si>
+  <si>
+    <t>92ffacdb5d781891a2ec19fe</t>
+  </si>
+  <si>
+    <t>776f59108b6fc73c5cb24af5</t>
+  </si>
+  <si>
+    <t>d4009cc5b4b9321d6048bd1e</t>
+  </si>
+  <si>
+    <t>dd5a8bde52281e471aae1b31</t>
+  </si>
+  <si>
+    <t>4bbad62f899c37c05f95dc65</t>
+  </si>
+  <si>
+    <t>726bb2a3c312c7cf793d6635</t>
+  </si>
+  <si>
+    <t>5e629c299a4adb39f4812ba0</t>
+  </si>
+  <si>
+    <t>69133a1d8bc96ddbd27f6a90</t>
+  </si>
+  <si>
+    <t>6cc66a0398f00b19a357689e</t>
+  </si>
+  <si>
+    <t>3223656b28064e27e49fb83c</t>
+  </si>
+  <si>
+    <t>b511a28f586eb8d271366d83</t>
+  </si>
+  <si>
+    <t>91127a76cb5d43f5514df740</t>
+  </si>
+  <si>
+    <t>36f38f0c623512140970a726</t>
+  </si>
+  <si>
+    <t>b8fa799b46fd55ee81439c2d</t>
+  </si>
+  <si>
+    <t>908488de50f985ec4cf12d04</t>
+  </si>
+  <si>
+    <t>f8da08e631fa07248edba0c3</t>
+  </si>
+  <si>
+    <t>eacef5dbc2eac63ce70e6307</t>
+  </si>
+  <si>
+    <t>ffa519f579ef37f2892b0157</t>
+  </si>
+  <si>
+    <t>20f9ea289c7d562c0cfe259b</t>
+  </si>
+  <si>
+    <t>a36cd50e1ffe1e7c72b82d51</t>
+  </si>
+  <si>
+    <t>a0fce2d3f2d813d2887720ff</t>
+  </si>
+  <si>
+    <t>4869fd10a7da9418844db277</t>
+  </si>
+  <si>
+    <t>c61ea7e639b2bfd24078f84d</t>
+  </si>
+  <si>
+    <t>66ae837db6b234c0c78864a0</t>
+  </si>
+  <si>
+    <t>d65c375eff8f1f2a66304580</t>
+  </si>
+  <si>
+    <t>8fe6e26b02aca4acb4a76e90</t>
+  </si>
+  <si>
+    <t>5331d04fbbcd92079dfb3800</t>
+  </si>
+  <si>
+    <t>ee2f53ac7ff244e42b7536d1</t>
+  </si>
+  <si>
+    <t>720ef4cf163dcdcc9b7a7416</t>
+  </si>
+  <si>
+    <t>9adeffb20b0d78833ce07be8</t>
+  </si>
+  <si>
+    <t>98ddde76bf9d7f4f4241b5fb</t>
+  </si>
+  <si>
+    <t>d541360bcc5b1f3f68d636f2</t>
+  </si>
+  <si>
+    <t>ec087498bd1bee7a576fa1bf</t>
+  </si>
+  <si>
+    <t>57b01ac4c1cf42643b1fc0a7</t>
+  </si>
+  <si>
+    <t>0b51efbcf640e82ffa9044fa</t>
+  </si>
+  <si>
+    <t>52ef184db8386bc87d07133e</t>
+  </si>
+  <si>
+    <t>4d51f6514632d467c2bb744a</t>
+  </si>
+  <si>
+    <t>b9ae572e4a272eb5b5f20528</t>
+  </si>
+  <si>
+    <t>9d59d2d96c2605eb1436d71a</t>
+  </si>
+  <si>
+    <t>54af7ebd6dd3b4337eb3dd22</t>
+  </si>
+  <si>
+    <t>b022de1fb18118aee26ea330</t>
+  </si>
+  <si>
+    <t>d9102f3d2e1e493ae906c684</t>
+  </si>
+  <si>
+    <t>c71f908a34be34718d511b22</t>
+  </si>
+  <si>
+    <t>25a35b154554b46233fcd53a</t>
+  </si>
+  <si>
+    <t>65cf6d25dbbffc0ddd6949d8</t>
+  </si>
+  <si>
+    <t>383b28d4433ca658b9c24e1e</t>
+  </si>
+  <si>
+    <t>9ec12a5f95a5b216ba501808</t>
+  </si>
+  <si>
+    <t>7d586b628febee64333e8954</t>
+  </si>
+  <si>
+    <t>4f22946cb84128f3104291b9</t>
+  </si>
+  <si>
+    <t>980c92f985d83c7ab7cc2c6e</t>
+  </si>
+  <si>
+    <t>94d1dd9d11c792009348331d</t>
+  </si>
+  <si>
+    <t>c8e7f1553bddc1fdcf406087</t>
+  </si>
+  <si>
+    <t>0f7c2b5bb657af881a2025b6</t>
+  </si>
+  <si>
+    <t>f5ed766374e478f41c9eb2eb</t>
+  </si>
+  <si>
+    <t>fe1f7a916919bea49609737f</t>
+  </si>
+  <si>
+    <t>9d383da24dfbf3e25d571ce9</t>
+  </si>
+  <si>
+    <t>43f4443539b6564ea27feb61</t>
+  </si>
+  <si>
+    <t>de17af04f2d5cf0c81401f6d</t>
+  </si>
+  <si>
+    <t>65e9e7b69594b4e44828c01a</t>
+  </si>
+  <si>
+    <t>cd42d9d9c4147d33facd0752</t>
+  </si>
+  <si>
+    <t>eefd6fa74cb657ac4fdd3bde</t>
+  </si>
+  <si>
+    <t>8383c72287d03495cbdff3e1</t>
+  </si>
+  <si>
+    <t>bfc916677f6a950957f2d509</t>
+  </si>
+  <si>
+    <t>49224aba29b4dcc65fa45bb2</t>
+  </si>
+  <si>
+    <t>2cdc19abea29df1540328ba3</t>
+  </si>
+  <si>
+    <t>b30e6eda7f99df975fce6820</t>
+  </si>
+  <si>
+    <t>623172025ee69bacae5c5c27</t>
+  </si>
+  <si>
+    <t>297722a065986463762d735d</t>
+  </si>
+  <si>
+    <t>393a9582ef2c8bab01f0bf4a</t>
+  </si>
+  <si>
+    <t>dc8c901b29bbcd942e603f59</t>
+  </si>
+  <si>
+    <t>e9fd85b9c135254f6a1c047e</t>
+  </si>
+  <si>
+    <t>819907bcdb0d71c56a061022</t>
+  </si>
+  <si>
+    <t>9a14810064844886de6ed9ae</t>
+  </si>
+  <si>
+    <t>7a73d9c57b59c0c33f13d16f</t>
   </si>
   <si>
     <t>Pending</t>

</xml_diff>